<commit_message>
Update báo cáo Theo Hoàng Trần
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao khach hang moi theo nhan vien/CRMRYYY1_Bao cao KH moi.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao khach hang moi theo nhan vien/CRMRYYY1_Bao cao KH moi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -3017,9 +3017,27 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3065,23 +3083,8 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3110,9 +3113,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3195,6 +3195,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3203,18 +3215,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3224,17 +3224,17 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3381,19 +3381,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1904040</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:colOff>1952625</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>105204</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3413,8 +3413,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="104775" y="742951"/>
-          <a:ext cx="8676315" cy="3581400"/>
+          <a:off x="0" y="1219200"/>
+          <a:ext cx="8829675" cy="3305604"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4225,65 +4225,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="139"/>
-      <c r="B1" s="139"/>
-      <c r="C1" s="141" t="s">
+      <c r="A1" s="145"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="140" t="s">
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="146" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140" t="s">
+      <c r="H1" s="146"/>
+      <c r="I1" s="146" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="140"/>
+      <c r="J1" s="146"/>
     </row>
     <row r="2" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A2" s="139"/>
-      <c r="B2" s="139"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="140" t="s">
+      <c r="A2" s="145"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="146" t="s">
         <v>154</v>
       </c>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
     </row>
     <row r="3" spans="1:18" ht="12.75" customHeight="1">
-      <c r="A3" s="139"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="136" t="s">
+      <c r="A3" s="145"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="142" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="137"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="143"/>
     </row>
     <row r="4" spans="1:18">
       <c r="H4" s="119"/>
     </row>
     <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="138"/>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="138"/>
-      <c r="I13" s="138"/>
-      <c r="J13" s="138"/>
+      <c r="A13" s="144"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
+      <c r="J13" s="144"/>
       <c r="K13" s="120"/>
       <c r="L13" s="120"/>
       <c r="M13" s="120"/>
@@ -4294,56 +4294,56 @@
       <c r="R13" s="120"/>
     </row>
     <row r="14" spans="1:18" ht="26.25">
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="134"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="134"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="134"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="134"/>
-      <c r="N14" s="134"/>
-      <c r="O14" s="134"/>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="134"/>
-      <c r="R14" s="134"/>
+      <c r="B14" s="138"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="138"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+      <c r="N14" s="138"/>
+      <c r="O14" s="138"/>
+      <c r="P14" s="138"/>
+      <c r="Q14" s="138"/>
+      <c r="R14" s="138"/>
     </row>
     <row r="15" spans="1:18" ht="26.25">
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
-      <c r="F15" s="134"/>
-      <c r="G15" s="134"/>
-      <c r="H15" s="134"/>
-      <c r="I15" s="134"/>
-      <c r="J15" s="134"/>
-      <c r="K15" s="134"/>
-      <c r="L15" s="134"/>
-      <c r="M15" s="134"/>
-      <c r="N15" s="134"/>
-      <c r="O15" s="134"/>
-      <c r="P15" s="134"/>
-      <c r="Q15" s="134"/>
-      <c r="R15" s="134"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
+      <c r="F15" s="138"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="138"/>
+      <c r="N15" s="138"/>
+      <c r="O15" s="138"/>
+      <c r="P15" s="138"/>
+      <c r="Q15" s="138"/>
+      <c r="R15" s="138"/>
     </row>
     <row r="16" spans="1:18" ht="26.25">
-      <c r="A16" s="135" t="s">
+      <c r="A16" s="141" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="135"/>
-      <c r="C16" s="135"/>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="135"/>
-      <c r="G16" s="135"/>
-      <c r="H16" s="135"/>
-      <c r="I16" s="135"/>
-      <c r="J16" s="135"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="141"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="141"/>
+      <c r="J16" s="141"/>
       <c r="K16" s="121"/>
       <c r="L16" s="121"/>
       <c r="M16" s="121"/>
@@ -4354,384 +4354,384 @@
       <c r="R16" s="121"/>
     </row>
     <row r="17" spans="1:195" ht="14.1" customHeight="1">
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="134"/>
-      <c r="H17" s="134"/>
-      <c r="I17" s="134"/>
-      <c r="J17" s="134"/>
-      <c r="K17" s="134"/>
-      <c r="L17" s="134"/>
-      <c r="M17" s="134"/>
-      <c r="N17" s="134"/>
-      <c r="O17" s="134"/>
-      <c r="P17" s="134"/>
-      <c r="Q17" s="134"/>
-      <c r="R17" s="134"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="138"/>
+      <c r="K17" s="138"/>
+      <c r="L17" s="138"/>
+      <c r="M17" s="138"/>
+      <c r="N17" s="138"/>
+      <c r="O17" s="138"/>
+      <c r="P17" s="138"/>
+      <c r="Q17" s="138"/>
+      <c r="R17" s="138"/>
     </row>
     <row r="18" spans="1:195" ht="26.25">
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="134"/>
-      <c r="K18" s="134"/>
-      <c r="L18" s="134"/>
-      <c r="M18" s="134"/>
-      <c r="N18" s="134"/>
-      <c r="O18" s="134"/>
-      <c r="P18" s="134"/>
-      <c r="Q18" s="134"/>
-      <c r="R18" s="134"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="138"/>
+      <c r="O18" s="138"/>
+      <c r="P18" s="138"/>
+      <c r="Q18" s="138"/>
+      <c r="R18" s="138"/>
     </row>
     <row r="19" spans="1:195" ht="23.25">
-      <c r="B19" s="151"/>
-      <c r="C19" s="151"/>
-      <c r="D19" s="151"/>
-      <c r="E19" s="151"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="151"/>
-      <c r="H19" s="151"/>
-      <c r="I19" s="151"/>
-      <c r="J19" s="151"/>
-      <c r="K19" s="151"/>
-      <c r="L19" s="151"/>
-      <c r="M19" s="151"/>
-      <c r="N19" s="151"/>
-      <c r="O19" s="151"/>
-      <c r="P19" s="151"/>
-      <c r="Q19" s="151"/>
-      <c r="R19" s="151"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="140"/>
+      <c r="I19" s="140"/>
+      <c r="J19" s="140"/>
+      <c r="K19" s="140"/>
+      <c r="L19" s="140"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="140"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="140"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="140"/>
     </row>
     <row r="20" spans="1:195" ht="26.25">
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
-      <c r="K20" s="134"/>
-      <c r="L20" s="134"/>
-      <c r="M20" s="134"/>
-      <c r="N20" s="134"/>
-      <c r="O20" s="134"/>
-      <c r="P20" s="134"/>
-      <c r="Q20" s="134"/>
-      <c r="R20" s="134"/>
+      <c r="B20" s="138"/>
+      <c r="C20" s="138"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="138"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="138"/>
+      <c r="L20" s="138"/>
+      <c r="M20" s="138"/>
+      <c r="N20" s="138"/>
+      <c r="O20" s="138"/>
+      <c r="P20" s="138"/>
+      <c r="Q20" s="138"/>
+      <c r="R20" s="138"/>
     </row>
     <row r="21" spans="1:195" ht="26.25">
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="134"/>
-      <c r="I21" s="134"/>
-      <c r="J21" s="134"/>
-      <c r="K21" s="134"/>
-      <c r="L21" s="134"/>
-      <c r="M21" s="134"/>
-      <c r="N21" s="134"/>
-      <c r="O21" s="134"/>
-      <c r="P21" s="134"/>
-      <c r="Q21" s="134"/>
-      <c r="R21" s="134"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="138"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="138"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="138"/>
+      <c r="N21" s="138"/>
+      <c r="O21" s="138"/>
+      <c r="P21" s="138"/>
+      <c r="Q21" s="138"/>
+      <c r="R21" s="138"/>
     </row>
     <row r="22" spans="1:195" ht="25.5">
-      <c r="B22" s="150"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="150"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="150"/>
-      <c r="L22" s="150"/>
-      <c r="M22" s="150"/>
-      <c r="N22" s="150"/>
-      <c r="O22" s="150"/>
-      <c r="P22" s="150"/>
-      <c r="Q22" s="150"/>
-      <c r="R22" s="150"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
+      <c r="J22" s="139"/>
+      <c r="K22" s="139"/>
+      <c r="L22" s="139"/>
+      <c r="M22" s="139"/>
+      <c r="N22" s="139"/>
+      <c r="O22" s="139"/>
+      <c r="P22" s="139"/>
+      <c r="Q22" s="139"/>
+      <c r="R22" s="139"/>
     </row>
     <row r="23" spans="1:195" ht="25.5">
-      <c r="B23" s="150"/>
-      <c r="C23" s="150"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="150"/>
-      <c r="F23" s="150"/>
-      <c r="G23" s="150"/>
-      <c r="H23" s="150"/>
-      <c r="I23" s="150"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="150"/>
-      <c r="L23" s="150"/>
-      <c r="M23" s="150"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="150"/>
-      <c r="P23" s="150"/>
-      <c r="Q23" s="150"/>
-      <c r="R23" s="150"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="139"/>
+      <c r="I23" s="139"/>
+      <c r="J23" s="139"/>
+      <c r="K23" s="139"/>
+      <c r="L23" s="139"/>
+      <c r="M23" s="139"/>
+      <c r="N23" s="139"/>
+      <c r="O23" s="139"/>
+      <c r="P23" s="139"/>
+      <c r="Q23" s="139"/>
+      <c r="R23" s="139"/>
     </row>
     <row r="25" spans="1:195" ht="11.25" customHeight="1"/>
     <row r="26" spans="1:195" ht="18">
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
-      <c r="H26" s="152"/>
-      <c r="I26" s="152"/>
-      <c r="J26" s="152"/>
-      <c r="K26" s="152"/>
-      <c r="L26" s="152"/>
-      <c r="M26" s="152"/>
-      <c r="N26" s="152"/>
-      <c r="O26" s="152"/>
-      <c r="P26" s="152"/>
-      <c r="Q26" s="152"/>
-      <c r="R26" s="152"/>
+      <c r="B26" s="136"/>
+      <c r="C26" s="136"/>
+      <c r="D26" s="136"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136"/>
+      <c r="K26" s="136"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="136"/>
+      <c r="N26" s="136"/>
+      <c r="O26" s="136"/>
+      <c r="P26" s="136"/>
+      <c r="Q26" s="136"/>
+      <c r="R26" s="136"/>
     </row>
     <row r="28" spans="1:195" ht="18">
-      <c r="B28" s="154"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
-      <c r="H28" s="154"/>
-      <c r="I28" s="154"/>
-      <c r="J28" s="154"/>
-      <c r="K28" s="154"/>
-      <c r="L28" s="154"/>
-      <c r="M28" s="154"/>
-      <c r="N28" s="154"/>
-      <c r="O28" s="154"/>
-      <c r="P28" s="154"/>
-      <c r="Q28" s="154"/>
-      <c r="R28" s="154"/>
-      <c r="S28" s="153"/>
-      <c r="T28" s="153"/>
-      <c r="U28" s="153"/>
-      <c r="V28" s="153"/>
-      <c r="W28" s="153"/>
-      <c r="X28" s="153"/>
-      <c r="Y28" s="153"/>
-      <c r="Z28" s="153"/>
-      <c r="AA28" s="153"/>
-      <c r="AB28" s="153"/>
-      <c r="AC28" s="153"/>
-      <c r="AD28" s="153"/>
-      <c r="AE28" s="153"/>
-      <c r="AF28" s="153"/>
-      <c r="AG28" s="153"/>
-      <c r="AH28" s="153"/>
-      <c r="AI28" s="153"/>
-      <c r="AJ28" s="153"/>
-      <c r="AK28" s="153"/>
-      <c r="AL28" s="153"/>
-      <c r="AM28" s="153"/>
-      <c r="AN28" s="153"/>
-      <c r="AO28" s="153"/>
-      <c r="AP28" s="153"/>
-      <c r="AQ28" s="153"/>
-      <c r="AR28" s="153"/>
-      <c r="AS28" s="153"/>
-      <c r="AT28" s="153"/>
-      <c r="AU28" s="153"/>
-      <c r="AV28" s="153"/>
-      <c r="AW28" s="153"/>
-      <c r="AX28" s="153"/>
-      <c r="AY28" s="153"/>
-      <c r="AZ28" s="153"/>
-      <c r="BA28" s="153"/>
-      <c r="BB28" s="153"/>
-      <c r="BC28" s="153"/>
-      <c r="BD28" s="153"/>
-      <c r="BE28" s="153"/>
-      <c r="BF28" s="153"/>
-      <c r="BG28" s="153"/>
-      <c r="BH28" s="153"/>
-      <c r="BI28" s="153"/>
-      <c r="BJ28" s="153"/>
-      <c r="BK28" s="153"/>
-      <c r="BL28" s="153"/>
-      <c r="BM28" s="153"/>
-      <c r="BN28" s="153"/>
-      <c r="BO28" s="153"/>
-      <c r="BP28" s="153"/>
-      <c r="BQ28" s="153"/>
-      <c r="BR28" s="153"/>
-      <c r="BS28" s="153"/>
-      <c r="BT28" s="153"/>
-      <c r="BU28" s="153"/>
-      <c r="BV28" s="153"/>
-      <c r="BW28" s="153"/>
-      <c r="BX28" s="153"/>
-      <c r="BY28" s="153"/>
-      <c r="BZ28" s="153"/>
-      <c r="CA28" s="153"/>
-      <c r="CB28" s="153"/>
-      <c r="CC28" s="153"/>
-      <c r="CD28" s="153"/>
-      <c r="CE28" s="153"/>
-      <c r="CF28" s="153"/>
-      <c r="CG28" s="153"/>
-      <c r="CH28" s="153"/>
-      <c r="CI28" s="153"/>
-      <c r="CJ28" s="153"/>
-      <c r="CK28" s="153"/>
-      <c r="CL28" s="153"/>
-      <c r="CM28" s="153"/>
-      <c r="CN28" s="153"/>
-      <c r="CO28" s="153"/>
-      <c r="CP28" s="153"/>
-      <c r="CQ28" s="153"/>
-      <c r="CR28" s="153"/>
-      <c r="CS28" s="153"/>
-      <c r="CT28" s="153"/>
-      <c r="CU28" s="153"/>
-      <c r="CV28" s="153"/>
-      <c r="CW28" s="153"/>
-      <c r="CX28" s="153"/>
-      <c r="CY28" s="153"/>
-      <c r="CZ28" s="153"/>
-      <c r="DA28" s="153"/>
-      <c r="DB28" s="153"/>
-      <c r="DC28" s="153"/>
-      <c r="DD28" s="153"/>
-      <c r="DE28" s="153"/>
-      <c r="DF28" s="153"/>
-      <c r="DG28" s="153"/>
-      <c r="DH28" s="153"/>
-      <c r="DI28" s="153"/>
-      <c r="DJ28" s="153"/>
-      <c r="DK28" s="153"/>
-      <c r="DL28" s="153"/>
-      <c r="DM28" s="153"/>
-      <c r="DN28" s="153"/>
-      <c r="DO28" s="153"/>
-      <c r="DP28" s="153"/>
-      <c r="DQ28" s="153"/>
-      <c r="DR28" s="153"/>
-      <c r="DS28" s="153"/>
-      <c r="DT28" s="153"/>
-      <c r="DU28" s="153"/>
-      <c r="DV28" s="153"/>
-      <c r="DW28" s="153"/>
-      <c r="DX28" s="153"/>
-      <c r="DY28" s="153"/>
-      <c r="DZ28" s="153"/>
-      <c r="EA28" s="153"/>
-      <c r="EB28" s="153"/>
-      <c r="EC28" s="153"/>
-      <c r="ED28" s="153"/>
-      <c r="EE28" s="153"/>
-      <c r="EF28" s="153"/>
-      <c r="EG28" s="153"/>
-      <c r="EH28" s="153"/>
-      <c r="EI28" s="153"/>
-      <c r="EJ28" s="153"/>
-      <c r="EK28" s="153"/>
-      <c r="EL28" s="153"/>
-      <c r="EM28" s="153"/>
-      <c r="EN28" s="153"/>
-      <c r="EO28" s="153"/>
-      <c r="EP28" s="153"/>
-      <c r="EQ28" s="153"/>
-      <c r="ER28" s="153"/>
-      <c r="ES28" s="153"/>
-      <c r="ET28" s="153"/>
-      <c r="EU28" s="153"/>
-      <c r="EV28" s="153"/>
-      <c r="EW28" s="153"/>
-      <c r="EX28" s="153"/>
-      <c r="EY28" s="153"/>
-      <c r="EZ28" s="153"/>
-      <c r="FA28" s="153"/>
-      <c r="FB28" s="153"/>
-      <c r="FC28" s="153"/>
-      <c r="FD28" s="153"/>
-      <c r="FE28" s="153"/>
-      <c r="FF28" s="153"/>
-      <c r="FG28" s="153"/>
-      <c r="FH28" s="153"/>
-      <c r="FI28" s="153"/>
-      <c r="FJ28" s="153"/>
-      <c r="FK28" s="153"/>
-      <c r="FL28" s="153"/>
-      <c r="FM28" s="153"/>
-      <c r="FN28" s="153"/>
-      <c r="FO28" s="153"/>
-      <c r="FP28" s="153"/>
-      <c r="FQ28" s="153"/>
-      <c r="FR28" s="153"/>
-      <c r="FS28" s="153"/>
-      <c r="FT28" s="153"/>
-      <c r="FU28" s="153"/>
-      <c r="FV28" s="153"/>
-      <c r="FW28" s="153"/>
-      <c r="FX28" s="153"/>
-      <c r="FY28" s="153"/>
-      <c r="FZ28" s="153"/>
-      <c r="GA28" s="153"/>
-      <c r="GB28" s="153"/>
-      <c r="GC28" s="153"/>
-      <c r="GD28" s="153"/>
-      <c r="GE28" s="153"/>
-      <c r="GF28" s="153"/>
-      <c r="GG28" s="153"/>
-      <c r="GH28" s="153"/>
-      <c r="GI28" s="153"/>
-      <c r="GJ28" s="153"/>
-      <c r="GK28" s="153"/>
-      <c r="GL28" s="153"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="137"/>
+      <c r="I28" s="137"/>
+      <c r="J28" s="137"/>
+      <c r="K28" s="137"/>
+      <c r="L28" s="137"/>
+      <c r="M28" s="137"/>
+      <c r="N28" s="137"/>
+      <c r="O28" s="137"/>
+      <c r="P28" s="137"/>
+      <c r="Q28" s="137"/>
+      <c r="R28" s="137"/>
+      <c r="S28" s="135"/>
+      <c r="T28" s="135"/>
+      <c r="U28" s="135"/>
+      <c r="V28" s="135"/>
+      <c r="W28" s="135"/>
+      <c r="X28" s="135"/>
+      <c r="Y28" s="135"/>
+      <c r="Z28" s="135"/>
+      <c r="AA28" s="135"/>
+      <c r="AB28" s="135"/>
+      <c r="AC28" s="135"/>
+      <c r="AD28" s="135"/>
+      <c r="AE28" s="135"/>
+      <c r="AF28" s="135"/>
+      <c r="AG28" s="135"/>
+      <c r="AH28" s="135"/>
+      <c r="AI28" s="135"/>
+      <c r="AJ28" s="135"/>
+      <c r="AK28" s="135"/>
+      <c r="AL28" s="135"/>
+      <c r="AM28" s="135"/>
+      <c r="AN28" s="135"/>
+      <c r="AO28" s="135"/>
+      <c r="AP28" s="135"/>
+      <c r="AQ28" s="135"/>
+      <c r="AR28" s="135"/>
+      <c r="AS28" s="135"/>
+      <c r="AT28" s="135"/>
+      <c r="AU28" s="135"/>
+      <c r="AV28" s="135"/>
+      <c r="AW28" s="135"/>
+      <c r="AX28" s="135"/>
+      <c r="AY28" s="135"/>
+      <c r="AZ28" s="135"/>
+      <c r="BA28" s="135"/>
+      <c r="BB28" s="135"/>
+      <c r="BC28" s="135"/>
+      <c r="BD28" s="135"/>
+      <c r="BE28" s="135"/>
+      <c r="BF28" s="135"/>
+      <c r="BG28" s="135"/>
+      <c r="BH28" s="135"/>
+      <c r="BI28" s="135"/>
+      <c r="BJ28" s="135"/>
+      <c r="BK28" s="135"/>
+      <c r="BL28" s="135"/>
+      <c r="BM28" s="135"/>
+      <c r="BN28" s="135"/>
+      <c r="BO28" s="135"/>
+      <c r="BP28" s="135"/>
+      <c r="BQ28" s="135"/>
+      <c r="BR28" s="135"/>
+      <c r="BS28" s="135"/>
+      <c r="BT28" s="135"/>
+      <c r="BU28" s="135"/>
+      <c r="BV28" s="135"/>
+      <c r="BW28" s="135"/>
+      <c r="BX28" s="135"/>
+      <c r="BY28" s="135"/>
+      <c r="BZ28" s="135"/>
+      <c r="CA28" s="135"/>
+      <c r="CB28" s="135"/>
+      <c r="CC28" s="135"/>
+      <c r="CD28" s="135"/>
+      <c r="CE28" s="135"/>
+      <c r="CF28" s="135"/>
+      <c r="CG28" s="135"/>
+      <c r="CH28" s="135"/>
+      <c r="CI28" s="135"/>
+      <c r="CJ28" s="135"/>
+      <c r="CK28" s="135"/>
+      <c r="CL28" s="135"/>
+      <c r="CM28" s="135"/>
+      <c r="CN28" s="135"/>
+      <c r="CO28" s="135"/>
+      <c r="CP28" s="135"/>
+      <c r="CQ28" s="135"/>
+      <c r="CR28" s="135"/>
+      <c r="CS28" s="135"/>
+      <c r="CT28" s="135"/>
+      <c r="CU28" s="135"/>
+      <c r="CV28" s="135"/>
+      <c r="CW28" s="135"/>
+      <c r="CX28" s="135"/>
+      <c r="CY28" s="135"/>
+      <c r="CZ28" s="135"/>
+      <c r="DA28" s="135"/>
+      <c r="DB28" s="135"/>
+      <c r="DC28" s="135"/>
+      <c r="DD28" s="135"/>
+      <c r="DE28" s="135"/>
+      <c r="DF28" s="135"/>
+      <c r="DG28" s="135"/>
+      <c r="DH28" s="135"/>
+      <c r="DI28" s="135"/>
+      <c r="DJ28" s="135"/>
+      <c r="DK28" s="135"/>
+      <c r="DL28" s="135"/>
+      <c r="DM28" s="135"/>
+      <c r="DN28" s="135"/>
+      <c r="DO28" s="135"/>
+      <c r="DP28" s="135"/>
+      <c r="DQ28" s="135"/>
+      <c r="DR28" s="135"/>
+      <c r="DS28" s="135"/>
+      <c r="DT28" s="135"/>
+      <c r="DU28" s="135"/>
+      <c r="DV28" s="135"/>
+      <c r="DW28" s="135"/>
+      <c r="DX28" s="135"/>
+      <c r="DY28" s="135"/>
+      <c r="DZ28" s="135"/>
+      <c r="EA28" s="135"/>
+      <c r="EB28" s="135"/>
+      <c r="EC28" s="135"/>
+      <c r="ED28" s="135"/>
+      <c r="EE28" s="135"/>
+      <c r="EF28" s="135"/>
+      <c r="EG28" s="135"/>
+      <c r="EH28" s="135"/>
+      <c r="EI28" s="135"/>
+      <c r="EJ28" s="135"/>
+      <c r="EK28" s="135"/>
+      <c r="EL28" s="135"/>
+      <c r="EM28" s="135"/>
+      <c r="EN28" s="135"/>
+      <c r="EO28" s="135"/>
+      <c r="EP28" s="135"/>
+      <c r="EQ28" s="135"/>
+      <c r="ER28" s="135"/>
+      <c r="ES28" s="135"/>
+      <c r="ET28" s="135"/>
+      <c r="EU28" s="135"/>
+      <c r="EV28" s="135"/>
+      <c r="EW28" s="135"/>
+      <c r="EX28" s="135"/>
+      <c r="EY28" s="135"/>
+      <c r="EZ28" s="135"/>
+      <c r="FA28" s="135"/>
+      <c r="FB28" s="135"/>
+      <c r="FC28" s="135"/>
+      <c r="FD28" s="135"/>
+      <c r="FE28" s="135"/>
+      <c r="FF28" s="135"/>
+      <c r="FG28" s="135"/>
+      <c r="FH28" s="135"/>
+      <c r="FI28" s="135"/>
+      <c r="FJ28" s="135"/>
+      <c r="FK28" s="135"/>
+      <c r="FL28" s="135"/>
+      <c r="FM28" s="135"/>
+      <c r="FN28" s="135"/>
+      <c r="FO28" s="135"/>
+      <c r="FP28" s="135"/>
+      <c r="FQ28" s="135"/>
+      <c r="FR28" s="135"/>
+      <c r="FS28" s="135"/>
+      <c r="FT28" s="135"/>
+      <c r="FU28" s="135"/>
+      <c r="FV28" s="135"/>
+      <c r="FW28" s="135"/>
+      <c r="FX28" s="135"/>
+      <c r="FY28" s="135"/>
+      <c r="FZ28" s="135"/>
+      <c r="GA28" s="135"/>
+      <c r="GB28" s="135"/>
+      <c r="GC28" s="135"/>
+      <c r="GD28" s="135"/>
+      <c r="GE28" s="135"/>
+      <c r="GF28" s="135"/>
+      <c r="GG28" s="135"/>
+      <c r="GH28" s="135"/>
+      <c r="GI28" s="135"/>
+      <c r="GJ28" s="135"/>
+      <c r="GK28" s="135"/>
+      <c r="GL28" s="135"/>
       <c r="GM28" s="122"/>
     </row>
     <row r="29" spans="1:195" ht="18">
-      <c r="B29" s="152"/>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="152"/>
-      <c r="J29" s="152"/>
-      <c r="K29" s="152"/>
-      <c r="L29" s="152"/>
-      <c r="M29" s="152"/>
-      <c r="N29" s="152"/>
-      <c r="O29" s="152"/>
-      <c r="P29" s="152"/>
-      <c r="Q29" s="152"/>
-      <c r="R29" s="152"/>
+      <c r="B29" s="136"/>
+      <c r="C29" s="136"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
+      <c r="G29" s="136"/>
+      <c r="H29" s="136"/>
+      <c r="I29" s="136"/>
+      <c r="J29" s="136"/>
+      <c r="K29" s="136"/>
+      <c r="L29" s="136"/>
+      <c r="M29" s="136"/>
+      <c r="N29" s="136"/>
+      <c r="O29" s="136"/>
+      <c r="P29" s="136"/>
+      <c r="Q29" s="136"/>
+      <c r="R29" s="136"/>
     </row>
     <row r="30" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A30" s="155"/>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
-      <c r="H30" s="155"/>
-      <c r="I30" s="155"/>
-      <c r="J30" s="155"/>
+      <c r="A30" s="134"/>
+      <c r="B30" s="134"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="134"/>
+      <c r="I30" s="134"/>
+      <c r="J30" s="134"/>
       <c r="K30" s="123"/>
       <c r="L30" s="123"/>
       <c r="M30" s="123"/>
@@ -4742,16 +4742,16 @@
       <c r="R30" s="123"/>
     </row>
     <row r="31" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A31" s="155"/>
-      <c r="B31" s="155"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="155"/>
-      <c r="E31" s="155"/>
-      <c r="F31" s="155"/>
-      <c r="G31" s="155"/>
-      <c r="H31" s="155"/>
-      <c r="I31" s="155"/>
-      <c r="J31" s="155"/>
+      <c r="A31" s="134"/>
+      <c r="B31" s="134"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="134"/>
+      <c r="I31" s="134"/>
+      <c r="J31" s="134"/>
       <c r="K31" s="123"/>
       <c r="L31" s="123"/>
       <c r="M31" s="123"/>
@@ -4763,28 +4763,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="DF28:DV28"/>
-    <mergeCell ref="DW28:EM28"/>
-    <mergeCell ref="EN28:FD28"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="FE28:FU28"/>
-    <mergeCell ref="FV28:GL28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="S28:X28"/>
-    <mergeCell ref="Y28:AO28"/>
-    <mergeCell ref="AP28:BF28"/>
-    <mergeCell ref="BG28:BW28"/>
-    <mergeCell ref="BX28:CN28"/>
-    <mergeCell ref="CO28:DE28"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B19:R19"/>
     <mergeCell ref="B14:R14"/>
     <mergeCell ref="B15:R15"/>
     <mergeCell ref="A16:J16"/>
@@ -4798,6 +4776,28 @@
     <mergeCell ref="C1:F3"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B20:R20"/>
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B19:R19"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="FE28:FU28"/>
+    <mergeCell ref="FV28:GL28"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="Y28:AO28"/>
+    <mergeCell ref="AP28:BF28"/>
+    <mergeCell ref="BG28:BW28"/>
+    <mergeCell ref="BX28:CN28"/>
+    <mergeCell ref="CO28:DE28"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="DF28:DV28"/>
+    <mergeCell ref="DW28:EM28"/>
+    <mergeCell ref="EN28:FD28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0" header="0" footer="0"/>
@@ -5352,10 +5352,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
+      <c r="B1" s="163"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -5382,8 +5382,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="162"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5425,14 +5425,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="163" t="s">
+      <c r="E4" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
+      <c r="F4" s="164"/>
+      <c r="G4" s="164"/>
+      <c r="H4" s="164"/>
+      <c r="I4" s="164"/>
+      <c r="J4" s="164"/>
     </row>
     <row r="5" spans="1:10" ht="24.75" customHeight="1">
       <c r="A5" s="40">
@@ -5447,14 +5447,14 @@
       <c r="D5" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="164" t="s">
+      <c r="E5" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5" s="156"/>
     </row>
     <row r="6" spans="1:10" ht="12.75">
       <c r="A6" s="92">
@@ -5481,12 +5481,12 @@
       </c>
       <c r="C7" s="80"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="158"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="158"/>
+      <c r="G7" s="158"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="159"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="94">
@@ -5497,12 +5497,12 @@
       </c>
       <c r="C8" s="80"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="160"/>
-      <c r="G8" s="160"/>
-      <c r="H8" s="160"/>
-      <c r="I8" s="160"/>
-      <c r="J8" s="161"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="161"/>
+      <c r="I8" s="161"/>
+      <c r="J8" s="162"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="95">
@@ -5513,12 +5513,12 @@
       </c>
       <c r="C9" s="80"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="158"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="158"/>
+      <c r="G9" s="158"/>
+      <c r="H9" s="158"/>
+      <c r="I9" s="158"/>
+      <c r="J9" s="159"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="96">
@@ -5529,12 +5529,12 @@
       </c>
       <c r="C10" s="80"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="156"/>
-      <c r="F10" s="157"/>
-      <c r="G10" s="157"/>
-      <c r="H10" s="157"/>
-      <c r="I10" s="157"/>
-      <c r="J10" s="158"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="158"/>
+      <c r="H10" s="158"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="159"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="97">
@@ -5545,12 +5545,12 @@
       </c>
       <c r="C11" s="80"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="156"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="157"/>
-      <c r="J11" s="158"/>
+      <c r="E11" s="157"/>
+      <c r="F11" s="158"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="158"/>
+      <c r="I11" s="158"/>
+      <c r="J11" s="159"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="98">
@@ -5561,12 +5561,12 @@
       </c>
       <c r="C12" s="80"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="156"/>
-      <c r="F12" s="157"/>
-      <c r="G12" s="157"/>
-      <c r="H12" s="157"/>
-      <c r="I12" s="157"/>
-      <c r="J12" s="158"/>
+      <c r="E12" s="157"/>
+      <c r="F12" s="158"/>
+      <c r="G12" s="158"/>
+      <c r="H12" s="158"/>
+      <c r="I12" s="158"/>
+      <c r="J12" s="159"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="99">
@@ -5577,12 +5577,12 @@
       </c>
       <c r="C13" s="80"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="156"/>
-      <c r="F13" s="157"/>
-      <c r="G13" s="157"/>
-      <c r="H13" s="157"/>
-      <c r="I13" s="157"/>
-      <c r="J13" s="158"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="158"/>
+      <c r="G13" s="158"/>
+      <c r="H13" s="158"/>
+      <c r="I13" s="158"/>
+      <c r="J13" s="159"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="100">
@@ -5593,12 +5593,12 @@
       </c>
       <c r="C14" s="80"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="156"/>
-      <c r="F14" s="157"/>
-      <c r="G14" s="157"/>
-      <c r="H14" s="157"/>
-      <c r="I14" s="157"/>
-      <c r="J14" s="158"/>
+      <c r="E14" s="157"/>
+      <c r="F14" s="158"/>
+      <c r="G14" s="158"/>
+      <c r="H14" s="158"/>
+      <c r="I14" s="158"/>
+      <c r="J14" s="159"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="40">
@@ -5609,12 +5609,12 @@
       </c>
       <c r="C15" s="80"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="165"/>
-      <c r="F15" s="165"/>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
-      <c r="J15" s="165"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="156"/>
+      <c r="G15" s="156"/>
+      <c r="H15" s="156"/>
+      <c r="I15" s="156"/>
+      <c r="J15" s="156"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="92">
@@ -5625,12 +5625,12 @@
       </c>
       <c r="C16" s="80"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="165"/>
-      <c r="G16" s="165"/>
-      <c r="H16" s="165"/>
-      <c r="I16" s="165"/>
-      <c r="J16" s="165"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="156"/>
+      <c r="H16" s="156"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="156"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="93">
@@ -5641,12 +5641,12 @@
       </c>
       <c r="C17" s="80"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="165"/>
-      <c r="F17" s="165"/>
-      <c r="G17" s="165"/>
-      <c r="H17" s="165"/>
-      <c r="I17" s="165"/>
-      <c r="J17" s="165"/>
+      <c r="E17" s="156"/>
+      <c r="F17" s="156"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="94">
@@ -5657,12 +5657,12 @@
       </c>
       <c r="C18" s="80"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
+      <c r="H18" s="156"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="156"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="95">
@@ -5673,12 +5673,12 @@
       </c>
       <c r="C19" s="80"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="165"/>
-      <c r="F19" s="165"/>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165"/>
-      <c r="J19" s="165"/>
+      <c r="E19" s="156"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="156"/>
+      <c r="H19" s="156"/>
+      <c r="I19" s="156"/>
+      <c r="J19" s="156"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="96">
@@ -5689,12 +5689,12 @@
       </c>
       <c r="C20" s="80"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="165"/>
-      <c r="F20" s="165"/>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165"/>
-      <c r="J20" s="165"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="97">
@@ -5705,12 +5705,12 @@
       </c>
       <c r="C21" s="80"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="165"/>
-      <c r="F21" s="165"/>
-      <c r="G21" s="165"/>
-      <c r="H21" s="165"/>
-      <c r="I21" s="165"/>
-      <c r="J21" s="165"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
+      <c r="H21" s="156"/>
+      <c r="I21" s="156"/>
+      <c r="J21" s="156"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="98">
@@ -5721,12 +5721,12 @@
       </c>
       <c r="C22" s="80"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="165"/>
-      <c r="F22" s="165"/>
-      <c r="G22" s="165"/>
-      <c r="H22" s="165"/>
-      <c r="I22" s="165"/>
-      <c r="J22" s="165"/>
+      <c r="E22" s="156"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="156"/>
+      <c r="H22" s="156"/>
+      <c r="I22" s="156"/>
+      <c r="J22" s="156"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="99">
@@ -5737,12 +5737,12 @@
       </c>
       <c r="C23" s="80"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="165"/>
-      <c r="F23" s="165"/>
-      <c r="G23" s="165"/>
-      <c r="H23" s="165"/>
-      <c r="I23" s="165"/>
-      <c r="J23" s="165"/>
+      <c r="E23" s="156"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="156"/>
+      <c r="H23" s="156"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="156"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="100">
@@ -5753,12 +5753,12 @@
       </c>
       <c r="C24" s="80"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="165"/>
-      <c r="F24" s="165"/>
-      <c r="G24" s="165"/>
-      <c r="H24" s="165"/>
-      <c r="I24" s="165"/>
-      <c r="J24" s="165"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
+      <c r="H24" s="156"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="40">
@@ -5769,12 +5769,12 @@
       </c>
       <c r="C25" s="80"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
-      <c r="H25" s="165"/>
-      <c r="I25" s="165"/>
-      <c r="J25" s="165"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="40">
@@ -5785,12 +5785,12 @@
       </c>
       <c r="C26" s="80"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="165"/>
-      <c r="F26" s="165"/>
-      <c r="G26" s="165"/>
-      <c r="H26" s="165"/>
-      <c r="I26" s="165"/>
-      <c r="J26" s="165"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="156"/>
+      <c r="H26" s="156"/>
+      <c r="I26" s="156"/>
+      <c r="J26" s="156"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="92">
@@ -5801,12 +5801,12 @@
       </c>
       <c r="C27" s="80"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="165"/>
-      <c r="J27" s="165"/>
+      <c r="E27" s="156"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="156"/>
+      <c r="H27" s="156"/>
+      <c r="I27" s="156"/>
+      <c r="J27" s="156"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="93">
@@ -5817,12 +5817,12 @@
       </c>
       <c r="C28" s="80"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="165"/>
-      <c r="F28" s="165"/>
-      <c r="G28" s="165"/>
-      <c r="H28" s="165"/>
-      <c r="I28" s="165"/>
-      <c r="J28" s="165"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="94">
@@ -5833,12 +5833,12 @@
       </c>
       <c r="C29" s="80"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="165"/>
-      <c r="F29" s="165"/>
-      <c r="G29" s="165"/>
-      <c r="H29" s="165"/>
-      <c r="I29" s="165"/>
-      <c r="J29" s="165"/>
+      <c r="E29" s="156"/>
+      <c r="F29" s="156"/>
+      <c r="G29" s="156"/>
+      <c r="H29" s="156"/>
+      <c r="I29" s="156"/>
+      <c r="J29" s="156"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="95">
@@ -5849,12 +5849,12 @@
       </c>
       <c r="C30" s="80"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
-      <c r="H30" s="165"/>
-      <c r="I30" s="165"/>
-      <c r="J30" s="165"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="156"/>
+      <c r="I30" s="156"/>
+      <c r="J30" s="156"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="96">
@@ -5865,12 +5865,12 @@
       </c>
       <c r="C31" s="80"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="165"/>
-      <c r="F31" s="165"/>
-      <c r="G31" s="165"/>
-      <c r="H31" s="165"/>
-      <c r="I31" s="165"/>
-      <c r="J31" s="165"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
+      <c r="H31" s="156"/>
+      <c r="I31" s="156"/>
+      <c r="J31" s="156"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="97">
@@ -5881,12 +5881,12 @@
       </c>
       <c r="C32" s="80"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="165"/>
-      <c r="F32" s="165"/>
-      <c r="G32" s="165"/>
-      <c r="H32" s="165"/>
-      <c r="I32" s="165"/>
-      <c r="J32" s="165"/>
+      <c r="E32" s="156"/>
+      <c r="F32" s="156"/>
+      <c r="G32" s="156"/>
+      <c r="H32" s="156"/>
+      <c r="I32" s="156"/>
+      <c r="J32" s="156"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="98">
@@ -5897,12 +5897,12 @@
       </c>
       <c r="C33" s="80"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="165"/>
-      <c r="F33" s="165"/>
-      <c r="G33" s="165"/>
-      <c r="H33" s="165"/>
-      <c r="I33" s="165"/>
-      <c r="J33" s="165"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="156"/>
+      <c r="H33" s="156"/>
+      <c r="I33" s="156"/>
+      <c r="J33" s="156"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="99">
@@ -5913,12 +5913,12 @@
       </c>
       <c r="C34" s="80"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="165"/>
-      <c r="F34" s="165"/>
-      <c r="G34" s="165"/>
-      <c r="H34" s="165"/>
-      <c r="I34" s="165"/>
-      <c r="J34" s="165"/>
+      <c r="E34" s="156"/>
+      <c r="F34" s="156"/>
+      <c r="G34" s="156"/>
+      <c r="H34" s="156"/>
+      <c r="I34" s="156"/>
+      <c r="J34" s="156"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="100">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="C35" s="80"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="165"/>
-      <c r="F35" s="165"/>
-      <c r="G35" s="165"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="165"/>
-      <c r="J35" s="165"/>
+      <c r="E35" s="156"/>
+      <c r="F35" s="156"/>
+      <c r="G35" s="156"/>
+      <c r="H35" s="156"/>
+      <c r="I35" s="156"/>
+      <c r="J35" s="156"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="40">
@@ -5945,12 +5945,12 @@
       </c>
       <c r="C36" s="80"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="165"/>
-      <c r="F36" s="165"/>
-      <c r="G36" s="165"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
-      <c r="J36" s="165"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="156"/>
+      <c r="H36" s="156"/>
+      <c r="I36" s="156"/>
+      <c r="J36" s="156"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="92">
@@ -5961,12 +5961,12 @@
       </c>
       <c r="C37" s="80"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="165"/>
-      <c r="F37" s="165"/>
-      <c r="G37" s="165"/>
-      <c r="H37" s="165"/>
-      <c r="I37" s="165"/>
-      <c r="J37" s="165"/>
+      <c r="E37" s="156"/>
+      <c r="F37" s="156"/>
+      <c r="G37" s="156"/>
+      <c r="H37" s="156"/>
+      <c r="I37" s="156"/>
+      <c r="J37" s="156"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="93">
@@ -5977,12 +5977,12 @@
       </c>
       <c r="C38" s="80"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="165"/>
-      <c r="F38" s="165"/>
-      <c r="G38" s="165"/>
-      <c r="H38" s="165"/>
-      <c r="I38" s="165"/>
-      <c r="J38" s="165"/>
+      <c r="E38" s="156"/>
+      <c r="F38" s="156"/>
+      <c r="G38" s="156"/>
+      <c r="H38" s="156"/>
+      <c r="I38" s="156"/>
+      <c r="J38" s="156"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="94">
@@ -5993,12 +5993,12 @@
       </c>
       <c r="C39" s="80"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="165"/>
-      <c r="F39" s="165"/>
-      <c r="G39" s="165"/>
-      <c r="H39" s="165"/>
-      <c r="I39" s="165"/>
-      <c r="J39" s="165"/>
+      <c r="E39" s="156"/>
+      <c r="F39" s="156"/>
+      <c r="G39" s="156"/>
+      <c r="H39" s="156"/>
+      <c r="I39" s="156"/>
+      <c r="J39" s="156"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="95">
@@ -6009,12 +6009,12 @@
       </c>
       <c r="C40" s="80"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="165"/>
-      <c r="F40" s="165"/>
-      <c r="G40" s="165"/>
-      <c r="H40" s="165"/>
-      <c r="I40" s="165"/>
-      <c r="J40" s="165"/>
+      <c r="E40" s="156"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="156"/>
+      <c r="H40" s="156"/>
+      <c r="I40" s="156"/>
+      <c r="J40" s="156"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="96">
@@ -6025,12 +6025,12 @@
       </c>
       <c r="C41" s="80"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="165"/>
-      <c r="F41" s="165"/>
-      <c r="G41" s="165"/>
-      <c r="H41" s="165"/>
-      <c r="I41" s="165"/>
-      <c r="J41" s="165"/>
+      <c r="E41" s="156"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="156"/>
+      <c r="H41" s="156"/>
+      <c r="I41" s="156"/>
+      <c r="J41" s="156"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="97">
@@ -6041,32 +6041,23 @@
       </c>
       <c r="C42" s="80"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="165"/>
-      <c r="F42" s="165"/>
-      <c r="G42" s="165"/>
-      <c r="H42" s="165"/>
-      <c r="I42" s="165"/>
-      <c r="J42" s="165"/>
+      <c r="E42" s="156"/>
+      <c r="F42" s="156"/>
+      <c r="G42" s="156"/>
+      <c r="H42" s="156"/>
+      <c r="I42" s="156"/>
+      <c r="J42" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -6082,14 +6073,23 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -6114,7 +6114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I12" sqref="I12:J43"/>
     </sheetView>
   </sheetViews>
@@ -6134,10 +6134,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
+      <c r="B1" s="163"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -6165,8 +6165,8 @@
       <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="162"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -6738,7 +6738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -6766,12 +6766,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
       <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6801,10 +6801,10 @@
       <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
       <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
@@ -9067,7 +9067,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="195" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="126"/>
@@ -9100,7 +9100,7 @@
       <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="199"/>
+      <c r="A2" s="196"/>
       <c r="B2" s="127"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
@@ -9146,15 +9146,15 @@
       <c r="E4" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="163" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="162"/>
-      <c r="H4" s="162" t="s">
+      <c r="G4" s="163"/>
+      <c r="H4" s="163" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="162"/>
-      <c r="J4" s="162"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
     </row>
     <row r="5" spans="1:12" s="34" customFormat="1" ht="25.5" customHeight="1">
       <c r="A5" s="33">
@@ -9168,15 +9168,15 @@
         <v>135</v>
       </c>
       <c r="E5" s="32"/>
-      <c r="F5" s="196" t="s">
+      <c r="F5" s="193" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="197"/>
-      <c r="H5" s="193" t="s">
+      <c r="G5" s="194"/>
+      <c r="H5" s="197" t="s">
         <v>210</v>
       </c>
-      <c r="I5" s="194"/>
-      <c r="J5" s="195"/>
+      <c r="I5" s="198"/>
+      <c r="J5" s="199"/>
     </row>
     <row r="6" spans="1:12" s="34" customFormat="1" ht="11.25">
       <c r="A6" s="33">
@@ -9186,11 +9186,11 @@
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
       <c r="E6" s="32"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="197"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="194"/>
-      <c r="J6" s="195"/>
+      <c r="F6" s="193"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="198"/>
+      <c r="J6" s="199"/>
     </row>
     <row r="7" spans="1:12" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A7" s="33">
@@ -9200,11 +9200,11 @@
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="196"/>
-      <c r="G7" s="197"/>
-      <c r="H7" s="193"/>
-      <c r="I7" s="194"/>
-      <c r="J7" s="195"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="194"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="198"/>
+      <c r="J7" s="199"/>
     </row>
     <row r="8" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="33">
@@ -9214,11 +9214,11 @@
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="196"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="193"/>
-      <c r="I8" s="194"/>
-      <c r="J8" s="195"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="198"/>
+      <c r="J8" s="199"/>
     </row>
     <row r="9" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="33">
@@ -9228,11 +9228,11 @@
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
-      <c r="F9" s="196"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="195"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="197"/>
+      <c r="I9" s="198"/>
+      <c r="J9" s="199"/>
     </row>
     <row r="10" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="33">
@@ -9242,11 +9242,11 @@
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="196"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="194"/>
-      <c r="J10" s="195"/>
+      <c r="F10" s="193"/>
+      <c r="G10" s="194"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="198"/>
+      <c r="J10" s="199"/>
     </row>
     <row r="11" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="33">
@@ -9256,11 +9256,11 @@
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="196"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="194"/>
-      <c r="J11" s="195"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="194"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="198"/>
+      <c r="J11" s="199"/>
     </row>
     <row r="12" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="33">
@@ -9270,11 +9270,11 @@
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="196"/>
-      <c r="G12" s="197"/>
-      <c r="H12" s="193"/>
-      <c r="I12" s="194"/>
-      <c r="J12" s="195"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="197"/>
+      <c r="I12" s="198"/>
+      <c r="J12" s="199"/>
     </row>
     <row r="13" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -9284,11 +9284,11 @@
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="196"/>
-      <c r="G13" s="197"/>
-      <c r="H13" s="193"/>
-      <c r="I13" s="194"/>
-      <c r="J13" s="195"/>
+      <c r="F13" s="193"/>
+      <c r="G13" s="194"/>
+      <c r="H13" s="197"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="199"/>
     </row>
     <row r="14" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -9298,11 +9298,11 @@
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="196"/>
-      <c r="G14" s="197"/>
-      <c r="H14" s="193"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="195"/>
+      <c r="F14" s="193"/>
+      <c r="G14" s="194"/>
+      <c r="H14" s="197"/>
+      <c r="I14" s="198"/>
+      <c r="J14" s="199"/>
     </row>
     <row r="15" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -9312,11 +9312,11 @@
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="196"/>
-      <c r="G15" s="197"/>
-      <c r="H15" s="193"/>
-      <c r="I15" s="194"/>
-      <c r="J15" s="195"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="194"/>
+      <c r="H15" s="197"/>
+      <c r="I15" s="198"/>
+      <c r="J15" s="199"/>
     </row>
     <row r="16" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="33">
@@ -9326,11 +9326,11 @@
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="32"/>
-      <c r="F16" s="196"/>
-      <c r="G16" s="197"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="194"/>
-      <c r="J16" s="195"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="194"/>
+      <c r="H16" s="197"/>
+      <c r="I16" s="198"/>
+      <c r="J16" s="199"/>
     </row>
     <row r="17" spans="1:18" s="34" customFormat="1" ht="11.25">
       <c r="A17" s="33">
@@ -9340,11 +9340,11 @@
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="32"/>
-      <c r="F17" s="196"/>
-      <c r="G17" s="197"/>
-      <c r="H17" s="193"/>
-      <c r="I17" s="194"/>
-      <c r="J17" s="195"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="194"/>
+      <c r="H17" s="197"/>
+      <c r="I17" s="198"/>
+      <c r="J17" s="199"/>
     </row>
     <row r="18" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -9354,11 +9354,11 @@
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="32"/>
-      <c r="F18" s="196"/>
-      <c r="G18" s="197"/>
-      <c r="H18" s="193"/>
-      <c r="I18" s="194"/>
-      <c r="J18" s="195"/>
+      <c r="F18" s="193"/>
+      <c r="G18" s="194"/>
+      <c r="H18" s="197"/>
+      <c r="I18" s="198"/>
+      <c r="J18" s="199"/>
     </row>
     <row r="19" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -9368,11 +9368,11 @@
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="32"/>
-      <c r="F19" s="196"/>
-      <c r="G19" s="197"/>
-      <c r="H19" s="193"/>
-      <c r="I19" s="194"/>
-      <c r="J19" s="195"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="194"/>
+      <c r="H19" s="197"/>
+      <c r="I19" s="198"/>
+      <c r="J19" s="199"/>
     </row>
     <row r="20" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="33">
@@ -9382,11 +9382,11 @@
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="196"/>
-      <c r="G20" s="197"/>
-      <c r="H20" s="193"/>
-      <c r="I20" s="194"/>
-      <c r="J20" s="195"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="194"/>
+      <c r="H20" s="197"/>
+      <c r="I20" s="198"/>
+      <c r="J20" s="199"/>
     </row>
     <row r="21" spans="1:18" s="34" customFormat="1" ht="11.25">
       <c r="A21" s="33">
@@ -9396,11 +9396,11 @@
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="196"/>
-      <c r="G21" s="197"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="194"/>
-      <c r="J21" s="195"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="194"/>
+      <c r="H21" s="197"/>
+      <c r="I21" s="198"/>
+      <c r="J21" s="199"/>
     </row>
     <row r="22" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
@@ -9410,11 +9410,11 @@
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="32"/>
-      <c r="F22" s="156"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="193"/>
-      <c r="I22" s="194"/>
-      <c r="J22" s="195"/>
+      <c r="F22" s="157"/>
+      <c r="G22" s="159"/>
+      <c r="H22" s="197"/>
+      <c r="I22" s="198"/>
+      <c r="J22" s="199"/>
     </row>
     <row r="23" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
@@ -9424,11 +9424,11 @@
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
-      <c r="F23" s="156"/>
-      <c r="G23" s="158"/>
-      <c r="H23" s="193"/>
-      <c r="I23" s="194"/>
-      <c r="J23" s="195"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="197"/>
+      <c r="I23" s="198"/>
+      <c r="J23" s="199"/>
     </row>
     <row r="24" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
@@ -9438,11 +9438,11 @@
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="32"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="193"/>
-      <c r="I24" s="194"/>
-      <c r="J24" s="195"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="197"/>
+      <c r="I24" s="198"/>
+      <c r="J24" s="199"/>
     </row>
     <row r="25" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
@@ -9452,11 +9452,11 @@
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="193"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="195"/>
+      <c r="F25" s="157"/>
+      <c r="G25" s="159"/>
+      <c r="H25" s="197"/>
+      <c r="I25" s="198"/>
+      <c r="J25" s="199"/>
     </row>
     <row r="26" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
@@ -9466,11 +9466,11 @@
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="158"/>
-      <c r="H26" s="193"/>
-      <c r="I26" s="194"/>
-      <c r="J26" s="195"/>
+      <c r="F26" s="157"/>
+      <c r="G26" s="159"/>
+      <c r="H26" s="197"/>
+      <c r="I26" s="198"/>
+      <c r="J26" s="199"/>
     </row>
     <row r="27" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
@@ -9480,11 +9480,11 @@
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="156"/>
-      <c r="G27" s="158"/>
-      <c r="H27" s="193"/>
-      <c r="I27" s="194"/>
-      <c r="J27" s="195"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="159"/>
+      <c r="H27" s="197"/>
+      <c r="I27" s="198"/>
+      <c r="J27" s="199"/>
     </row>
     <row r="28" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
@@ -9494,11 +9494,11 @@
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="158"/>
-      <c r="H28" s="193"/>
-      <c r="I28" s="194"/>
-      <c r="J28" s="195"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="197"/>
+      <c r="I28" s="198"/>
+      <c r="J28" s="199"/>
     </row>
     <row r="29" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33">
@@ -9508,11 +9508,11 @@
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
-      <c r="F29" s="156"/>
-      <c r="G29" s="158"/>
-      <c r="H29" s="193"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="195"/>
+      <c r="F29" s="157"/>
+      <c r="G29" s="159"/>
+      <c r="H29" s="197"/>
+      <c r="I29" s="198"/>
+      <c r="J29" s="199"/>
     </row>
     <row r="30" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A30" s="33">
@@ -9522,11 +9522,11 @@
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="156"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="194"/>
-      <c r="J30" s="195"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="197"/>
+      <c r="I30" s="198"/>
+      <c r="J30" s="199"/>
     </row>
     <row r="31" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A31" s="33">
@@ -9536,11 +9536,11 @@
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="193"/>
-      <c r="I31" s="194"/>
-      <c r="J31" s="195"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="197"/>
+      <c r="I31" s="198"/>
+      <c r="J31" s="199"/>
     </row>
     <row r="32" spans="1:18" ht="11.25">
       <c r="A32" s="33">
@@ -9550,11 +9550,11 @@
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
-      <c r="F32" s="156"/>
-      <c r="G32" s="158"/>
-      <c r="H32" s="193"/>
-      <c r="I32" s="194"/>
-      <c r="J32" s="195"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="159"/>
+      <c r="H32" s="197"/>
+      <c r="I32" s="198"/>
+      <c r="J32" s="199"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
@@ -9571,11 +9571,11 @@
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="156"/>
-      <c r="G33" s="158"/>
-      <c r="H33" s="193"/>
-      <c r="I33" s="194"/>
-      <c r="J33" s="195"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="159"/>
+      <c r="H33" s="197"/>
+      <c r="I33" s="198"/>
+      <c r="J33" s="199"/>
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
@@ -9592,11 +9592,11 @@
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
-      <c r="F34" s="156"/>
-      <c r="G34" s="158"/>
-      <c r="H34" s="193"/>
-      <c r="I34" s="194"/>
-      <c r="J34" s="195"/>
+      <c r="F34" s="157"/>
+      <c r="G34" s="159"/>
+      <c r="H34" s="197"/>
+      <c r="I34" s="198"/>
+      <c r="J34" s="199"/>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
@@ -9613,11 +9613,11 @@
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
-      <c r="F35" s="156"/>
-      <c r="G35" s="158"/>
-      <c r="H35" s="193"/>
-      <c r="I35" s="194"/>
-      <c r="J35" s="195"/>
+      <c r="F35" s="157"/>
+      <c r="G35" s="159"/>
+      <c r="H35" s="197"/>
+      <c r="I35" s="198"/>
+      <c r="J35" s="199"/>
       <c r="L35" s="22"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
@@ -9634,11 +9634,11 @@
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="32"/>
-      <c r="F36" s="156"/>
-      <c r="G36" s="158"/>
-      <c r="H36" s="193"/>
-      <c r="I36" s="194"/>
-      <c r="J36" s="195"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="159"/>
+      <c r="H36" s="197"/>
+      <c r="I36" s="198"/>
+      <c r="J36" s="199"/>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
@@ -9655,11 +9655,11 @@
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
-      <c r="F37" s="156"/>
-      <c r="G37" s="158"/>
-      <c r="H37" s="193"/>
-      <c r="I37" s="194"/>
-      <c r="J37" s="195"/>
+      <c r="F37" s="157"/>
+      <c r="G37" s="159"/>
+      <c r="H37" s="197"/>
+      <c r="I37" s="198"/>
+      <c r="J37" s="199"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
@@ -9676,11 +9676,11 @@
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="32"/>
-      <c r="F38" s="156"/>
-      <c r="G38" s="158"/>
-      <c r="H38" s="193"/>
-      <c r="I38" s="194"/>
-      <c r="J38" s="195"/>
+      <c r="F38" s="157"/>
+      <c r="G38" s="159"/>
+      <c r="H38" s="197"/>
+      <c r="I38" s="198"/>
+      <c r="J38" s="199"/>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
@@ -9697,11 +9697,11 @@
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="156"/>
-      <c r="G39" s="158"/>
-      <c r="H39" s="193"/>
-      <c r="I39" s="194"/>
-      <c r="J39" s="195"/>
+      <c r="F39" s="157"/>
+      <c r="G39" s="159"/>
+      <c r="H39" s="197"/>
+      <c r="I39" s="198"/>
+      <c r="J39" s="199"/>
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
@@ -9718,11 +9718,11 @@
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="32"/>
-      <c r="F40" s="156"/>
-      <c r="G40" s="158"/>
-      <c r="H40" s="193"/>
-      <c r="I40" s="194"/>
-      <c r="J40" s="195"/>
+      <c r="F40" s="157"/>
+      <c r="G40" s="159"/>
+      <c r="H40" s="197"/>
+      <c r="I40" s="198"/>
+      <c r="J40" s="199"/>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
@@ -9739,11 +9739,11 @@
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
-      <c r="F41" s="156"/>
-      <c r="G41" s="158"/>
-      <c r="H41" s="193"/>
-      <c r="I41" s="194"/>
-      <c r="J41" s="195"/>
+      <c r="F41" s="157"/>
+      <c r="G41" s="159"/>
+      <c r="H41" s="197"/>
+      <c r="I41" s="198"/>
+      <c r="J41" s="199"/>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
@@ -9760,11 +9760,11 @@
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="32"/>
-      <c r="F42" s="156"/>
-      <c r="G42" s="158"/>
-      <c r="H42" s="193"/>
-      <c r="I42" s="194"/>
-      <c r="J42" s="195"/>
+      <c r="F42" s="157"/>
+      <c r="G42" s="159"/>
+      <c r="H42" s="197"/>
+      <c r="I42" s="198"/>
+      <c r="J42" s="199"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
@@ -9781,11 +9781,11 @@
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="32"/>
-      <c r="F43" s="156"/>
-      <c r="G43" s="158"/>
-      <c r="H43" s="193"/>
-      <c r="I43" s="194"/>
-      <c r="J43" s="195"/>
+      <c r="F43" s="157"/>
+      <c r="G43" s="159"/>
+      <c r="H43" s="197"/>
+      <c r="I43" s="198"/>
+      <c r="J43" s="199"/>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
@@ -9802,11 +9802,11 @@
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
       <c r="E44" s="32"/>
-      <c r="F44" s="156"/>
-      <c r="G44" s="158"/>
-      <c r="H44" s="193"/>
-      <c r="I44" s="194"/>
-      <c r="J44" s="195"/>
+      <c r="F44" s="157"/>
+      <c r="G44" s="159"/>
+      <c r="H44" s="197"/>
+      <c r="I44" s="198"/>
+      <c r="J44" s="199"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
@@ -9823,11 +9823,11 @@
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
       <c r="E45" s="32"/>
-      <c r="F45" s="156"/>
-      <c r="G45" s="158"/>
-      <c r="H45" s="193"/>
-      <c r="I45" s="194"/>
-      <c r="J45" s="195"/>
+      <c r="F45" s="157"/>
+      <c r="G45" s="159"/>
+      <c r="H45" s="197"/>
+      <c r="I45" s="198"/>
+      <c r="J45" s="199"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
@@ -9844,11 +9844,11 @@
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
       <c r="E46" s="32"/>
-      <c r="F46" s="156"/>
-      <c r="G46" s="158"/>
-      <c r="H46" s="193"/>
-      <c r="I46" s="194"/>
-      <c r="J46" s="195"/>
+      <c r="F46" s="157"/>
+      <c r="G46" s="159"/>
+      <c r="H46" s="197"/>
+      <c r="I46" s="198"/>
+      <c r="J46" s="199"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
@@ -9865,11 +9865,11 @@
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="32"/>
-      <c r="F47" s="156"/>
-      <c r="G47" s="158"/>
-      <c r="H47" s="193"/>
-      <c r="I47" s="194"/>
-      <c r="J47" s="195"/>
+      <c r="F47" s="157"/>
+      <c r="G47" s="159"/>
+      <c r="H47" s="197"/>
+      <c r="I47" s="198"/>
+      <c r="J47" s="199"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
@@ -9886,11 +9886,11 @@
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="32"/>
-      <c r="F48" s="156"/>
-      <c r="G48" s="158"/>
-      <c r="H48" s="193"/>
-      <c r="I48" s="194"/>
-      <c r="J48" s="195"/>
+      <c r="F48" s="157"/>
+      <c r="G48" s="159"/>
+      <c r="H48" s="197"/>
+      <c r="I48" s="198"/>
+      <c r="J48" s="199"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
@@ -9907,11 +9907,11 @@
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
-      <c r="F49" s="156"/>
-      <c r="G49" s="158"/>
-      <c r="H49" s="193"/>
-      <c r="I49" s="194"/>
-      <c r="J49" s="195"/>
+      <c r="F49" s="157"/>
+      <c r="G49" s="159"/>
+      <c r="H49" s="197"/>
+      <c r="I49" s="198"/>
+      <c r="J49" s="199"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
@@ -9928,11 +9928,11 @@
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="32"/>
-      <c r="F50" s="156"/>
-      <c r="G50" s="158"/>
-      <c r="H50" s="193"/>
-      <c r="I50" s="194"/>
-      <c r="J50" s="195"/>
+      <c r="F50" s="157"/>
+      <c r="G50" s="159"/>
+      <c r="H50" s="197"/>
+      <c r="I50" s="198"/>
+      <c r="J50" s="199"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
@@ -9949,11 +9949,11 @@
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="32"/>
-      <c r="F51" s="156"/>
-      <c r="G51" s="158"/>
-      <c r="H51" s="193"/>
-      <c r="I51" s="194"/>
-      <c r="J51" s="195"/>
+      <c r="F51" s="157"/>
+      <c r="G51" s="159"/>
+      <c r="H51" s="197"/>
+      <c r="I51" s="198"/>
+      <c r="J51" s="199"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
@@ -9970,11 +9970,11 @@
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="32"/>
-      <c r="F52" s="156"/>
-      <c r="G52" s="158"/>
-      <c r="H52" s="193"/>
-      <c r="I52" s="194"/>
-      <c r="J52" s="195"/>
+      <c r="F52" s="157"/>
+      <c r="G52" s="159"/>
+      <c r="H52" s="197"/>
+      <c r="I52" s="198"/>
+      <c r="J52" s="199"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
@@ -9991,11 +9991,11 @@
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="156"/>
-      <c r="G53" s="158"/>
-      <c r="H53" s="193"/>
-      <c r="I53" s="194"/>
-      <c r="J53" s="195"/>
+      <c r="F53" s="157"/>
+      <c r="G53" s="159"/>
+      <c r="H53" s="197"/>
+      <c r="I53" s="198"/>
+      <c r="J53" s="199"/>
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
@@ -10012,11 +10012,11 @@
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="32"/>
-      <c r="F54" s="156"/>
-      <c r="G54" s="158"/>
-      <c r="H54" s="193"/>
-      <c r="I54" s="194"/>
-      <c r="J54" s="195"/>
+      <c r="F54" s="157"/>
+      <c r="G54" s="159"/>
+      <c r="H54" s="197"/>
+      <c r="I54" s="198"/>
+      <c r="J54" s="199"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
@@ -10033,11 +10033,11 @@
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="32"/>
-      <c r="F55" s="156"/>
-      <c r="G55" s="158"/>
-      <c r="H55" s="193"/>
-      <c r="I55" s="194"/>
-      <c r="J55" s="195"/>
+      <c r="F55" s="157"/>
+      <c r="G55" s="159"/>
+      <c r="H55" s="197"/>
+      <c r="I55" s="198"/>
+      <c r="J55" s="199"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
@@ -10054,11 +10054,11 @@
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
       <c r="E56" s="32"/>
-      <c r="F56" s="156"/>
-      <c r="G56" s="158"/>
-      <c r="H56" s="193"/>
-      <c r="I56" s="194"/>
-      <c r="J56" s="195"/>
+      <c r="F56" s="157"/>
+      <c r="G56" s="159"/>
+      <c r="H56" s="197"/>
+      <c r="I56" s="198"/>
+      <c r="J56" s="199"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
@@ -10070,25 +10070,80 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="107">
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="H55:J55"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
@@ -10103,80 +10158,25 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H19:J19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="H55:J55"/>
-    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E56">
@@ -10222,23 +10222,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
       <c r="H1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="203" t="str">
+      <c r="I1" s="206" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="J1" s="203"/>
+      <c r="J1" s="206"/>
       <c r="K1" s="26" t="s">
         <v>3</v>
       </c>
@@ -10263,21 +10263,21 @@
       <c r="T1" s="52"/>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
       <c r="H2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="203" t="str">
+      <c r="I2" s="206" t="str">
         <f>'Update History'!D2</f>
         <v>ASSOFT - CRM</v>
       </c>
-      <c r="J2" s="203"/>
+      <c r="J2" s="206"/>
       <c r="K2" s="26" t="s">
         <v>49</v>
       </c>
@@ -10441,7 +10441,7 @@
       <c r="O7" s="90"/>
       <c r="P7" s="77"/>
       <c r="Q7" s="76"/>
-      <c r="R7" s="204"/>
+      <c r="R7" s="203"/>
       <c r="S7" s="64"/>
       <c r="T7" s="64"/>
     </row>
@@ -10465,7 +10465,7 @@
       <c r="O8" s="90"/>
       <c r="P8" s="77"/>
       <c r="Q8" s="76"/>
-      <c r="R8" s="205"/>
+      <c r="R8" s="204"/>
       <c r="S8" s="64"/>
       <c r="T8" s="64"/>
     </row>
@@ -10489,7 +10489,7 @@
       <c r="O9" s="90"/>
       <c r="P9" s="77"/>
       <c r="Q9" s="76"/>
-      <c r="R9" s="206"/>
+      <c r="R9" s="205"/>
       <c r="S9" s="64"/>
       <c r="T9" s="64"/>
     </row>
@@ -10513,7 +10513,7 @@
       <c r="O10" s="90"/>
       <c r="P10" s="77"/>
       <c r="Q10" s="76"/>
-      <c r="R10" s="204"/>
+      <c r="R10" s="203"/>
       <c r="S10" s="64"/>
       <c r="T10" s="64"/>
     </row>
@@ -10537,7 +10537,7 @@
       <c r="O11" s="90"/>
       <c r="P11" s="77"/>
       <c r="Q11" s="76"/>
-      <c r="R11" s="205"/>
+      <c r="R11" s="204"/>
       <c r="S11" s="64"/>
       <c r="T11" s="64"/>
     </row>
@@ -10561,7 +10561,7 @@
       <c r="O12" s="86"/>
       <c r="P12" s="77"/>
       <c r="Q12" s="76"/>
-      <c r="R12" s="205"/>
+      <c r="R12" s="204"/>
       <c r="S12" s="64"/>
       <c r="T12" s="64"/>
     </row>
@@ -10585,7 +10585,7 @@
       <c r="O13" s="86"/>
       <c r="P13" s="77"/>
       <c r="Q13" s="76"/>
-      <c r="R13" s="206"/>
+      <c r="R13" s="205"/>
       <c r="S13" s="64"/>
       <c r="T13" s="64"/>
     </row>
@@ -12477,11 +12477,81 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="96">
-    <mergeCell ref="J88:M88"/>
-    <mergeCell ref="J89:M89"/>
-    <mergeCell ref="J90:M90"/>
-    <mergeCell ref="J91:M91"/>
-    <mergeCell ref="J92:M92"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J93:M93"/>
+    <mergeCell ref="J94:M94"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J78:M78"/>
+    <mergeCell ref="J79:M79"/>
+    <mergeCell ref="J80:M80"/>
+    <mergeCell ref="J81:M81"/>
+    <mergeCell ref="J82:M82"/>
+    <mergeCell ref="J83:M83"/>
+    <mergeCell ref="J84:M84"/>
+    <mergeCell ref="J85:M85"/>
+    <mergeCell ref="J86:M86"/>
+    <mergeCell ref="J69:M69"/>
+    <mergeCell ref="J70:M70"/>
+    <mergeCell ref="J71:M71"/>
+    <mergeCell ref="J72:M72"/>
+    <mergeCell ref="J73:M73"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="J76:M76"/>
     <mergeCell ref="J77:M77"/>
     <mergeCell ref="J60:M60"/>
     <mergeCell ref="R7:R9"/>
@@ -12498,81 +12568,11 @@
     <mergeCell ref="J51:M51"/>
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J72:M72"/>
-    <mergeCell ref="J73:M73"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="J93:M93"/>
-    <mergeCell ref="J94:M94"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J78:M78"/>
-    <mergeCell ref="J79:M79"/>
-    <mergeCell ref="J80:M80"/>
-    <mergeCell ref="J81:M81"/>
-    <mergeCell ref="J82:M82"/>
-    <mergeCell ref="J83:M83"/>
-    <mergeCell ref="J84:M84"/>
-    <mergeCell ref="J85:M85"/>
-    <mergeCell ref="J86:M86"/>
-    <mergeCell ref="J69:M69"/>
-    <mergeCell ref="J70:M70"/>
-    <mergeCell ref="J71:M71"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J88:M88"/>
+    <mergeCell ref="J89:M89"/>
+    <mergeCell ref="J90:M90"/>
+    <mergeCell ref="J91:M91"/>
+    <mergeCell ref="J92:M92"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="P1048467:P1048576 P5:P94"/>
@@ -12618,10 +12618,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
+      <c r="B1" s="163"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -12649,8 +12649,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="162"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13718,10 +13718,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
+      <c r="B1" s="163"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13749,8 +13749,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="162"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Chỉnh sữa lại nội dung sau khi review
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao khach hang moi theo nhan vien/CRMRYYY1_Bao cao KH moi.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao khach hang moi theo nhan vien/CRMRYYY1_Bao cao KH moi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -1404,7 +1404,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="218">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2110,46 +2110,76 @@
     <t>@SQL0001</t>
   </si>
   <si>
-    <t>EXEC CRMP10104(
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Nhận tham số @DivisionID từ màn hình CRMFXXX1 để mở báo cáo CRMRYYY1</t>
+  </si>
+  <si>
+    <t>Click In từ màn hình CRMFXXX1</t>
+  </si>
+  <si>
+    <t>Thực thi @SQL0001 để in báo cáo Khách hàng mới theo nhân viên</t>
+  </si>
+  <si>
+    <t>Báo cáo KH mới theo nhân viên
+-&gt; In
+-&gt; Báo cáo khách hàng mới theo nhân viên</t>
+  </si>
+  <si>
+    <t>DivisionID</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXEC CRMP10104(
  @DivisionID       VARCHAR(50),  
-  @DivisionIDList    NVARCHAR(2000),  
-  @FromMonth        INT,
-  @FromYear          INT,
-  @ToMonth           INT,
-  @ToYear           INT,
+  @DivisionIDList    NVARCHAR(2000), 
   @FromDate         DATETIME,
   @ToDate           DATETIME,
   @IsDate           TINYINT,
-  @UserID  VARCHAR(50))</t>
-  </si>
-  <si>
-    <t>@DivisionID @DivisionIDList @FromMonth @FromYear @ToMonth @ToYear @FromDate @ToDate   @IsDate    @UserID</t>
-  </si>
-  <si>
-    <t>Biến môi trường @DivisionIDList @FromMonth @FromYear @ToMonth @ToYear @FromDate @ToDate   @IsDate       Biến môi trường</t>
-  </si>
-  <si>
-    <t>Click In</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>Nhận tham số từ màn hình CRMFXXX1 để load báo cáo khách hàng theo nhân viên</t>
-  </si>
-  <si>
-    <t>Nhận tham số @DivisionID từ màn hình CRMFXXX1 để mở báo cáo CRMRYYY1</t>
-  </si>
-  <si>
-    <t>Click In từ màn hình CRMFXXX1</t>
-  </si>
-  <si>
-    <t>Thực thi @SQL0001 để in báo cáo Khách hàng mới theo nhân viên</t>
-  </si>
-  <si>
-    <t>Báo cáo KH mới theo nhân viên
--&gt; In
--&gt; Báo cáo khách hàng mới theo nhân viên</t>
+@CheckBox1 TINYINT,
+@FromAccountID       Varchar(50),
+  @ToAccountID         Varchar(50),
+@CheckBox2 TINYINT,
+  @FromEmployeeID           Varchar(50),
+  @ToEmployeeID           Varchar(50),
+  @UserID  VARCHAR(50),
+@PageNumber INT,
+@PageSize INT)
+</t>
+  </si>
+  <si>
+    <t>@DivisionID @DivisionIDList  @FromDate @ToDate   @IsDate  
+@CheckBox1
+@FromAccountID @ToAccountID 
+@CheckBox2 @FromEmployeeID@ToEmployeeID @UserID
+@PageNumber
+@PageSize</t>
+  </si>
+  <si>
+    <t>Biến môi trường @@DivisionIDList  @@FromDate @@ToDate   @@IsDate 
+0,1 
+@@FromAccountID @@ToAccountID
+0,1 @@FromEmployeeID @@ToEmployeeID Biến môi trường
+@@PageNumber
+@@PageSize</t>
+  </si>
+  <si>
+    <t>Click BttnView</t>
+  </si>
+  <si>
+    <t>thực thi @SQL0005 để load báo cáo khách hàng theo nhân viên xem trước khi in</t>
+  </si>
+  <si>
+    <t>Group Theo DivisionID</t>
+  </si>
+  <si>
+    <t>Group theo SalesManID</t>
+  </si>
+  <si>
+    <t>SalesManID</t>
   </si>
 </sst>
 </file>
@@ -3004,115 +3034,115 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3195,6 +3225,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3206,15 +3245,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3224,6 +3254,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3232,9 +3265,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3381,19 +3411,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>105204</xdr:rowOff>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="6" name="Picture 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3413,8 +3443,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="1219200"/>
-          <a:ext cx="8829675" cy="3305604"/>
+          <a:off x="66675" y="1285875"/>
+          <a:ext cx="8515350" cy="3600450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4225,65 +4255,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="145"/>
-      <c r="B1" s="145"/>
-      <c r="C1" s="147" t="s">
+      <c r="A1" s="139"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="141" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="146" t="s">
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="140" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146" t="s">
+      <c r="H1" s="140"/>
+      <c r="I1" s="140" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="146"/>
+      <c r="J1" s="140"/>
     </row>
     <row r="2" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="146" t="s">
+      <c r="A2" s="139"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="140" t="s">
         <v>154</v>
       </c>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
     </row>
     <row r="3" spans="1:18" ht="12.75" customHeight="1">
-      <c r="A3" s="145"/>
-      <c r="B3" s="145"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="142" t="s">
+      <c r="A3" s="139"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="136" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="143"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="143"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="137"/>
     </row>
     <row r="4" spans="1:18">
       <c r="H4" s="119"/>
     </row>
     <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="144"/>
-      <c r="B13" s="144"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="144"/>
-      <c r="E13" s="144"/>
-      <c r="F13" s="144"/>
-      <c r="G13" s="144"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
-      <c r="J13" s="144"/>
+      <c r="A13" s="138"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
       <c r="K13" s="120"/>
       <c r="L13" s="120"/>
       <c r="M13" s="120"/>
@@ -4294,56 +4324,56 @@
       <c r="R13" s="120"/>
     </row>
     <row r="14" spans="1:18" ht="26.25">
-      <c r="B14" s="138"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="138"/>
-      <c r="J14" s="138"/>
-      <c r="K14" s="138"/>
-      <c r="L14" s="138"/>
-      <c r="M14" s="138"/>
-      <c r="N14" s="138"/>
-      <c r="O14" s="138"/>
-      <c r="P14" s="138"/>
-      <c r="Q14" s="138"/>
-      <c r="R14" s="138"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="134"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="134"/>
+      <c r="M14" s="134"/>
+      <c r="N14" s="134"/>
+      <c r="O14" s="134"/>
+      <c r="P14" s="134"/>
+      <c r="Q14" s="134"/>
+      <c r="R14" s="134"/>
     </row>
     <row r="15" spans="1:18" ht="26.25">
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="138"/>
-      <c r="I15" s="138"/>
-      <c r="J15" s="138"/>
-      <c r="K15" s="138"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="138"/>
-      <c r="N15" s="138"/>
-      <c r="O15" s="138"/>
-      <c r="P15" s="138"/>
-      <c r="Q15" s="138"/>
-      <c r="R15" s="138"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="134"/>
+      <c r="K15" s="134"/>
+      <c r="L15" s="134"/>
+      <c r="M15" s="134"/>
+      <c r="N15" s="134"/>
+      <c r="O15" s="134"/>
+      <c r="P15" s="134"/>
+      <c r="Q15" s="134"/>
+      <c r="R15" s="134"/>
     </row>
     <row r="16" spans="1:18" ht="26.25">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="135" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="141"/>
-      <c r="F16" s="141"/>
-      <c r="G16" s="141"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="141"/>
+      <c r="B16" s="135"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="135"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="135"/>
       <c r="K16" s="121"/>
       <c r="L16" s="121"/>
       <c r="M16" s="121"/>
@@ -4354,384 +4384,384 @@
       <c r="R16" s="121"/>
     </row>
     <row r="17" spans="1:195" ht="14.1" customHeight="1">
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="138"/>
-      <c r="H17" s="138"/>
-      <c r="I17" s="138"/>
-      <c r="J17" s="138"/>
-      <c r="K17" s="138"/>
-      <c r="L17" s="138"/>
-      <c r="M17" s="138"/>
-      <c r="N17" s="138"/>
-      <c r="O17" s="138"/>
-      <c r="P17" s="138"/>
-      <c r="Q17" s="138"/>
-      <c r="R17" s="138"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
+      <c r="F17" s="134"/>
+      <c r="G17" s="134"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="134"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="134"/>
+      <c r="L17" s="134"/>
+      <c r="M17" s="134"/>
+      <c r="N17" s="134"/>
+      <c r="O17" s="134"/>
+      <c r="P17" s="134"/>
+      <c r="Q17" s="134"/>
+      <c r="R17" s="134"/>
     </row>
     <row r="18" spans="1:195" ht="26.25">
-      <c r="B18" s="138"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="138"/>
-      <c r="I18" s="138"/>
-      <c r="J18" s="138"/>
-      <c r="K18" s="138"/>
-      <c r="L18" s="138"/>
-      <c r="M18" s="138"/>
-      <c r="N18" s="138"/>
-      <c r="O18" s="138"/>
-      <c r="P18" s="138"/>
-      <c r="Q18" s="138"/>
-      <c r="R18" s="138"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="134"/>
+      <c r="G18" s="134"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="134"/>
+      <c r="J18" s="134"/>
+      <c r="K18" s="134"/>
+      <c r="L18" s="134"/>
+      <c r="M18" s="134"/>
+      <c r="N18" s="134"/>
+      <c r="O18" s="134"/>
+      <c r="P18" s="134"/>
+      <c r="Q18" s="134"/>
+      <c r="R18" s="134"/>
     </row>
     <row r="19" spans="1:195" ht="23.25">
-      <c r="B19" s="140"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="140"/>
-      <c r="I19" s="140"/>
-      <c r="J19" s="140"/>
-      <c r="K19" s="140"/>
-      <c r="L19" s="140"/>
-      <c r="M19" s="140"/>
-      <c r="N19" s="140"/>
-      <c r="O19" s="140"/>
-      <c r="P19" s="140"/>
-      <c r="Q19" s="140"/>
-      <c r="R19" s="140"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="151"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
+      <c r="K19" s="151"/>
+      <c r="L19" s="151"/>
+      <c r="M19" s="151"/>
+      <c r="N19" s="151"/>
+      <c r="O19" s="151"/>
+      <c r="P19" s="151"/>
+      <c r="Q19" s="151"/>
+      <c r="R19" s="151"/>
     </row>
     <row r="20" spans="1:195" ht="26.25">
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="138"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="138"/>
-      <c r="K20" s="138"/>
-      <c r="L20" s="138"/>
-      <c r="M20" s="138"/>
-      <c r="N20" s="138"/>
-      <c r="O20" s="138"/>
-      <c r="P20" s="138"/>
-      <c r="Q20" s="138"/>
-      <c r="R20" s="138"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="134"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="134"/>
+      <c r="J20" s="134"/>
+      <c r="K20" s="134"/>
+      <c r="L20" s="134"/>
+      <c r="M20" s="134"/>
+      <c r="N20" s="134"/>
+      <c r="O20" s="134"/>
+      <c r="P20" s="134"/>
+      <c r="Q20" s="134"/>
+      <c r="R20" s="134"/>
     </row>
     <row r="21" spans="1:195" ht="26.25">
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="138"/>
-      <c r="I21" s="138"/>
-      <c r="J21" s="138"/>
-      <c r="K21" s="138"/>
-      <c r="L21" s="138"/>
-      <c r="M21" s="138"/>
-      <c r="N21" s="138"/>
-      <c r="O21" s="138"/>
-      <c r="P21" s="138"/>
-      <c r="Q21" s="138"/>
-      <c r="R21" s="138"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="134"/>
+      <c r="G21" s="134"/>
+      <c r="H21" s="134"/>
+      <c r="I21" s="134"/>
+      <c r="J21" s="134"/>
+      <c r="K21" s="134"/>
+      <c r="L21" s="134"/>
+      <c r="M21" s="134"/>
+      <c r="N21" s="134"/>
+      <c r="O21" s="134"/>
+      <c r="P21" s="134"/>
+      <c r="Q21" s="134"/>
+      <c r="R21" s="134"/>
     </row>
     <row r="22" spans="1:195" ht="25.5">
-      <c r="B22" s="139"/>
-      <c r="C22" s="139"/>
-      <c r="D22" s="139"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="139"/>
-      <c r="G22" s="139"/>
-      <c r="H22" s="139"/>
-      <c r="I22" s="139"/>
-      <c r="J22" s="139"/>
-      <c r="K22" s="139"/>
-      <c r="L22" s="139"/>
-      <c r="M22" s="139"/>
-      <c r="N22" s="139"/>
-      <c r="O22" s="139"/>
-      <c r="P22" s="139"/>
-      <c r="Q22" s="139"/>
-      <c r="R22" s="139"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
+      <c r="H22" s="150"/>
+      <c r="I22" s="150"/>
+      <c r="J22" s="150"/>
+      <c r="K22" s="150"/>
+      <c r="L22" s="150"/>
+      <c r="M22" s="150"/>
+      <c r="N22" s="150"/>
+      <c r="O22" s="150"/>
+      <c r="P22" s="150"/>
+      <c r="Q22" s="150"/>
+      <c r="R22" s="150"/>
     </row>
     <row r="23" spans="1:195" ht="25.5">
-      <c r="B23" s="139"/>
-      <c r="C23" s="139"/>
-      <c r="D23" s="139"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="139"/>
-      <c r="G23" s="139"/>
-      <c r="H23" s="139"/>
-      <c r="I23" s="139"/>
-      <c r="J23" s="139"/>
-      <c r="K23" s="139"/>
-      <c r="L23" s="139"/>
-      <c r="M23" s="139"/>
-      <c r="N23" s="139"/>
-      <c r="O23" s="139"/>
-      <c r="P23" s="139"/>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
+      <c r="B23" s="150"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="150"/>
+      <c r="E23" s="150"/>
+      <c r="F23" s="150"/>
+      <c r="G23" s="150"/>
+      <c r="H23" s="150"/>
+      <c r="I23" s="150"/>
+      <c r="J23" s="150"/>
+      <c r="K23" s="150"/>
+      <c r="L23" s="150"/>
+      <c r="M23" s="150"/>
+      <c r="N23" s="150"/>
+      <c r="O23" s="150"/>
+      <c r="P23" s="150"/>
+      <c r="Q23" s="150"/>
+      <c r="R23" s="150"/>
     </row>
     <row r="25" spans="1:195" ht="11.25" customHeight="1"/>
     <row r="26" spans="1:195" ht="18">
-      <c r="B26" s="136"/>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="136"/>
-      <c r="G26" s="136"/>
-      <c r="H26" s="136"/>
-      <c r="I26" s="136"/>
-      <c r="J26" s="136"/>
-      <c r="K26" s="136"/>
-      <c r="L26" s="136"/>
-      <c r="M26" s="136"/>
-      <c r="N26" s="136"/>
-      <c r="O26" s="136"/>
-      <c r="P26" s="136"/>
-      <c r="Q26" s="136"/>
-      <c r="R26" s="136"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
+      <c r="H26" s="152"/>
+      <c r="I26" s="152"/>
+      <c r="J26" s="152"/>
+      <c r="K26" s="152"/>
+      <c r="L26" s="152"/>
+      <c r="M26" s="152"/>
+      <c r="N26" s="152"/>
+      <c r="O26" s="152"/>
+      <c r="P26" s="152"/>
+      <c r="Q26" s="152"/>
+      <c r="R26" s="152"/>
     </row>
     <row r="28" spans="1:195" ht="18">
-      <c r="B28" s="137"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
-      <c r="H28" s="137"/>
-      <c r="I28" s="137"/>
-      <c r="J28" s="137"/>
-      <c r="K28" s="137"/>
-      <c r="L28" s="137"/>
-      <c r="M28" s="137"/>
-      <c r="N28" s="137"/>
-      <c r="O28" s="137"/>
-      <c r="P28" s="137"/>
-      <c r="Q28" s="137"/>
-      <c r="R28" s="137"/>
-      <c r="S28" s="135"/>
-      <c r="T28" s="135"/>
-      <c r="U28" s="135"/>
-      <c r="V28" s="135"/>
-      <c r="W28" s="135"/>
-      <c r="X28" s="135"/>
-      <c r="Y28" s="135"/>
-      <c r="Z28" s="135"/>
-      <c r="AA28" s="135"/>
-      <c r="AB28" s="135"/>
-      <c r="AC28" s="135"/>
-      <c r="AD28" s="135"/>
-      <c r="AE28" s="135"/>
-      <c r="AF28" s="135"/>
-      <c r="AG28" s="135"/>
-      <c r="AH28" s="135"/>
-      <c r="AI28" s="135"/>
-      <c r="AJ28" s="135"/>
-      <c r="AK28" s="135"/>
-      <c r="AL28" s="135"/>
-      <c r="AM28" s="135"/>
-      <c r="AN28" s="135"/>
-      <c r="AO28" s="135"/>
-      <c r="AP28" s="135"/>
-      <c r="AQ28" s="135"/>
-      <c r="AR28" s="135"/>
-      <c r="AS28" s="135"/>
-      <c r="AT28" s="135"/>
-      <c r="AU28" s="135"/>
-      <c r="AV28" s="135"/>
-      <c r="AW28" s="135"/>
-      <c r="AX28" s="135"/>
-      <c r="AY28" s="135"/>
-      <c r="AZ28" s="135"/>
-      <c r="BA28" s="135"/>
-      <c r="BB28" s="135"/>
-      <c r="BC28" s="135"/>
-      <c r="BD28" s="135"/>
-      <c r="BE28" s="135"/>
-      <c r="BF28" s="135"/>
-      <c r="BG28" s="135"/>
-      <c r="BH28" s="135"/>
-      <c r="BI28" s="135"/>
-      <c r="BJ28" s="135"/>
-      <c r="BK28" s="135"/>
-      <c r="BL28" s="135"/>
-      <c r="BM28" s="135"/>
-      <c r="BN28" s="135"/>
-      <c r="BO28" s="135"/>
-      <c r="BP28" s="135"/>
-      <c r="BQ28" s="135"/>
-      <c r="BR28" s="135"/>
-      <c r="BS28" s="135"/>
-      <c r="BT28" s="135"/>
-      <c r="BU28" s="135"/>
-      <c r="BV28" s="135"/>
-      <c r="BW28" s="135"/>
-      <c r="BX28" s="135"/>
-      <c r="BY28" s="135"/>
-      <c r="BZ28" s="135"/>
-      <c r="CA28" s="135"/>
-      <c r="CB28" s="135"/>
-      <c r="CC28" s="135"/>
-      <c r="CD28" s="135"/>
-      <c r="CE28" s="135"/>
-      <c r="CF28" s="135"/>
-      <c r="CG28" s="135"/>
-      <c r="CH28" s="135"/>
-      <c r="CI28" s="135"/>
-      <c r="CJ28" s="135"/>
-      <c r="CK28" s="135"/>
-      <c r="CL28" s="135"/>
-      <c r="CM28" s="135"/>
-      <c r="CN28" s="135"/>
-      <c r="CO28" s="135"/>
-      <c r="CP28" s="135"/>
-      <c r="CQ28" s="135"/>
-      <c r="CR28" s="135"/>
-      <c r="CS28" s="135"/>
-      <c r="CT28" s="135"/>
-      <c r="CU28" s="135"/>
-      <c r="CV28" s="135"/>
-      <c r="CW28" s="135"/>
-      <c r="CX28" s="135"/>
-      <c r="CY28" s="135"/>
-      <c r="CZ28" s="135"/>
-      <c r="DA28" s="135"/>
-      <c r="DB28" s="135"/>
-      <c r="DC28" s="135"/>
-      <c r="DD28" s="135"/>
-      <c r="DE28" s="135"/>
-      <c r="DF28" s="135"/>
-      <c r="DG28" s="135"/>
-      <c r="DH28" s="135"/>
-      <c r="DI28" s="135"/>
-      <c r="DJ28" s="135"/>
-      <c r="DK28" s="135"/>
-      <c r="DL28" s="135"/>
-      <c r="DM28" s="135"/>
-      <c r="DN28" s="135"/>
-      <c r="DO28" s="135"/>
-      <c r="DP28" s="135"/>
-      <c r="DQ28" s="135"/>
-      <c r="DR28" s="135"/>
-      <c r="DS28" s="135"/>
-      <c r="DT28" s="135"/>
-      <c r="DU28" s="135"/>
-      <c r="DV28" s="135"/>
-      <c r="DW28" s="135"/>
-      <c r="DX28" s="135"/>
-      <c r="DY28" s="135"/>
-      <c r="DZ28" s="135"/>
-      <c r="EA28" s="135"/>
-      <c r="EB28" s="135"/>
-      <c r="EC28" s="135"/>
-      <c r="ED28" s="135"/>
-      <c r="EE28" s="135"/>
-      <c r="EF28" s="135"/>
-      <c r="EG28" s="135"/>
-      <c r="EH28" s="135"/>
-      <c r="EI28" s="135"/>
-      <c r="EJ28" s="135"/>
-      <c r="EK28" s="135"/>
-      <c r="EL28" s="135"/>
-      <c r="EM28" s="135"/>
-      <c r="EN28" s="135"/>
-      <c r="EO28" s="135"/>
-      <c r="EP28" s="135"/>
-      <c r="EQ28" s="135"/>
-      <c r="ER28" s="135"/>
-      <c r="ES28" s="135"/>
-      <c r="ET28" s="135"/>
-      <c r="EU28" s="135"/>
-      <c r="EV28" s="135"/>
-      <c r="EW28" s="135"/>
-      <c r="EX28" s="135"/>
-      <c r="EY28" s="135"/>
-      <c r="EZ28" s="135"/>
-      <c r="FA28" s="135"/>
-      <c r="FB28" s="135"/>
-      <c r="FC28" s="135"/>
-      <c r="FD28" s="135"/>
-      <c r="FE28" s="135"/>
-      <c r="FF28" s="135"/>
-      <c r="FG28" s="135"/>
-      <c r="FH28" s="135"/>
-      <c r="FI28" s="135"/>
-      <c r="FJ28" s="135"/>
-      <c r="FK28" s="135"/>
-      <c r="FL28" s="135"/>
-      <c r="FM28" s="135"/>
-      <c r="FN28" s="135"/>
-      <c r="FO28" s="135"/>
-      <c r="FP28" s="135"/>
-      <c r="FQ28" s="135"/>
-      <c r="FR28" s="135"/>
-      <c r="FS28" s="135"/>
-      <c r="FT28" s="135"/>
-      <c r="FU28" s="135"/>
-      <c r="FV28" s="135"/>
-      <c r="FW28" s="135"/>
-      <c r="FX28" s="135"/>
-      <c r="FY28" s="135"/>
-      <c r="FZ28" s="135"/>
-      <c r="GA28" s="135"/>
-      <c r="GB28" s="135"/>
-      <c r="GC28" s="135"/>
-      <c r="GD28" s="135"/>
-      <c r="GE28" s="135"/>
-      <c r="GF28" s="135"/>
-      <c r="GG28" s="135"/>
-      <c r="GH28" s="135"/>
-      <c r="GI28" s="135"/>
-      <c r="GJ28" s="135"/>
-      <c r="GK28" s="135"/>
-      <c r="GL28" s="135"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
+      <c r="H28" s="154"/>
+      <c r="I28" s="154"/>
+      <c r="J28" s="154"/>
+      <c r="K28" s="154"/>
+      <c r="L28" s="154"/>
+      <c r="M28" s="154"/>
+      <c r="N28" s="154"/>
+      <c r="O28" s="154"/>
+      <c r="P28" s="154"/>
+      <c r="Q28" s="154"/>
+      <c r="R28" s="154"/>
+      <c r="S28" s="153"/>
+      <c r="T28" s="153"/>
+      <c r="U28" s="153"/>
+      <c r="V28" s="153"/>
+      <c r="W28" s="153"/>
+      <c r="X28" s="153"/>
+      <c r="Y28" s="153"/>
+      <c r="Z28" s="153"/>
+      <c r="AA28" s="153"/>
+      <c r="AB28" s="153"/>
+      <c r="AC28" s="153"/>
+      <c r="AD28" s="153"/>
+      <c r="AE28" s="153"/>
+      <c r="AF28" s="153"/>
+      <c r="AG28" s="153"/>
+      <c r="AH28" s="153"/>
+      <c r="AI28" s="153"/>
+      <c r="AJ28" s="153"/>
+      <c r="AK28" s="153"/>
+      <c r="AL28" s="153"/>
+      <c r="AM28" s="153"/>
+      <c r="AN28" s="153"/>
+      <c r="AO28" s="153"/>
+      <c r="AP28" s="153"/>
+      <c r="AQ28" s="153"/>
+      <c r="AR28" s="153"/>
+      <c r="AS28" s="153"/>
+      <c r="AT28" s="153"/>
+      <c r="AU28" s="153"/>
+      <c r="AV28" s="153"/>
+      <c r="AW28" s="153"/>
+      <c r="AX28" s="153"/>
+      <c r="AY28" s="153"/>
+      <c r="AZ28" s="153"/>
+      <c r="BA28" s="153"/>
+      <c r="BB28" s="153"/>
+      <c r="BC28" s="153"/>
+      <c r="BD28" s="153"/>
+      <c r="BE28" s="153"/>
+      <c r="BF28" s="153"/>
+      <c r="BG28" s="153"/>
+      <c r="BH28" s="153"/>
+      <c r="BI28" s="153"/>
+      <c r="BJ28" s="153"/>
+      <c r="BK28" s="153"/>
+      <c r="BL28" s="153"/>
+      <c r="BM28" s="153"/>
+      <c r="BN28" s="153"/>
+      <c r="BO28" s="153"/>
+      <c r="BP28" s="153"/>
+      <c r="BQ28" s="153"/>
+      <c r="BR28" s="153"/>
+      <c r="BS28" s="153"/>
+      <c r="BT28" s="153"/>
+      <c r="BU28" s="153"/>
+      <c r="BV28" s="153"/>
+      <c r="BW28" s="153"/>
+      <c r="BX28" s="153"/>
+      <c r="BY28" s="153"/>
+      <c r="BZ28" s="153"/>
+      <c r="CA28" s="153"/>
+      <c r="CB28" s="153"/>
+      <c r="CC28" s="153"/>
+      <c r="CD28" s="153"/>
+      <c r="CE28" s="153"/>
+      <c r="CF28" s="153"/>
+      <c r="CG28" s="153"/>
+      <c r="CH28" s="153"/>
+      <c r="CI28" s="153"/>
+      <c r="CJ28" s="153"/>
+      <c r="CK28" s="153"/>
+      <c r="CL28" s="153"/>
+      <c r="CM28" s="153"/>
+      <c r="CN28" s="153"/>
+      <c r="CO28" s="153"/>
+      <c r="CP28" s="153"/>
+      <c r="CQ28" s="153"/>
+      <c r="CR28" s="153"/>
+      <c r="CS28" s="153"/>
+      <c r="CT28" s="153"/>
+      <c r="CU28" s="153"/>
+      <c r="CV28" s="153"/>
+      <c r="CW28" s="153"/>
+      <c r="CX28" s="153"/>
+      <c r="CY28" s="153"/>
+      <c r="CZ28" s="153"/>
+      <c r="DA28" s="153"/>
+      <c r="DB28" s="153"/>
+      <c r="DC28" s="153"/>
+      <c r="DD28" s="153"/>
+      <c r="DE28" s="153"/>
+      <c r="DF28" s="153"/>
+      <c r="DG28" s="153"/>
+      <c r="DH28" s="153"/>
+      <c r="DI28" s="153"/>
+      <c r="DJ28" s="153"/>
+      <c r="DK28" s="153"/>
+      <c r="DL28" s="153"/>
+      <c r="DM28" s="153"/>
+      <c r="DN28" s="153"/>
+      <c r="DO28" s="153"/>
+      <c r="DP28" s="153"/>
+      <c r="DQ28" s="153"/>
+      <c r="DR28" s="153"/>
+      <c r="DS28" s="153"/>
+      <c r="DT28" s="153"/>
+      <c r="DU28" s="153"/>
+      <c r="DV28" s="153"/>
+      <c r="DW28" s="153"/>
+      <c r="DX28" s="153"/>
+      <c r="DY28" s="153"/>
+      <c r="DZ28" s="153"/>
+      <c r="EA28" s="153"/>
+      <c r="EB28" s="153"/>
+      <c r="EC28" s="153"/>
+      <c r="ED28" s="153"/>
+      <c r="EE28" s="153"/>
+      <c r="EF28" s="153"/>
+      <c r="EG28" s="153"/>
+      <c r="EH28" s="153"/>
+      <c r="EI28" s="153"/>
+      <c r="EJ28" s="153"/>
+      <c r="EK28" s="153"/>
+      <c r="EL28" s="153"/>
+      <c r="EM28" s="153"/>
+      <c r="EN28" s="153"/>
+      <c r="EO28" s="153"/>
+      <c r="EP28" s="153"/>
+      <c r="EQ28" s="153"/>
+      <c r="ER28" s="153"/>
+      <c r="ES28" s="153"/>
+      <c r="ET28" s="153"/>
+      <c r="EU28" s="153"/>
+      <c r="EV28" s="153"/>
+      <c r="EW28" s="153"/>
+      <c r="EX28" s="153"/>
+      <c r="EY28" s="153"/>
+      <c r="EZ28" s="153"/>
+      <c r="FA28" s="153"/>
+      <c r="FB28" s="153"/>
+      <c r="FC28" s="153"/>
+      <c r="FD28" s="153"/>
+      <c r="FE28" s="153"/>
+      <c r="FF28" s="153"/>
+      <c r="FG28" s="153"/>
+      <c r="FH28" s="153"/>
+      <c r="FI28" s="153"/>
+      <c r="FJ28" s="153"/>
+      <c r="FK28" s="153"/>
+      <c r="FL28" s="153"/>
+      <c r="FM28" s="153"/>
+      <c r="FN28" s="153"/>
+      <c r="FO28" s="153"/>
+      <c r="FP28" s="153"/>
+      <c r="FQ28" s="153"/>
+      <c r="FR28" s="153"/>
+      <c r="FS28" s="153"/>
+      <c r="FT28" s="153"/>
+      <c r="FU28" s="153"/>
+      <c r="FV28" s="153"/>
+      <c r="FW28" s="153"/>
+      <c r="FX28" s="153"/>
+      <c r="FY28" s="153"/>
+      <c r="FZ28" s="153"/>
+      <c r="GA28" s="153"/>
+      <c r="GB28" s="153"/>
+      <c r="GC28" s="153"/>
+      <c r="GD28" s="153"/>
+      <c r="GE28" s="153"/>
+      <c r="GF28" s="153"/>
+      <c r="GG28" s="153"/>
+      <c r="GH28" s="153"/>
+      <c r="GI28" s="153"/>
+      <c r="GJ28" s="153"/>
+      <c r="GK28" s="153"/>
+      <c r="GL28" s="153"/>
       <c r="GM28" s="122"/>
     </row>
     <row r="29" spans="1:195" ht="18">
-      <c r="B29" s="136"/>
-      <c r="C29" s="136"/>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="136"/>
-      <c r="G29" s="136"/>
-      <c r="H29" s="136"/>
-      <c r="I29" s="136"/>
-      <c r="J29" s="136"/>
-      <c r="K29" s="136"/>
-      <c r="L29" s="136"/>
-      <c r="M29" s="136"/>
-      <c r="N29" s="136"/>
-      <c r="O29" s="136"/>
-      <c r="P29" s="136"/>
-      <c r="Q29" s="136"/>
-      <c r="R29" s="136"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="152"/>
+      <c r="J29" s="152"/>
+      <c r="K29" s="152"/>
+      <c r="L29" s="152"/>
+      <c r="M29" s="152"/>
+      <c r="N29" s="152"/>
+      <c r="O29" s="152"/>
+      <c r="P29" s="152"/>
+      <c r="Q29" s="152"/>
+      <c r="R29" s="152"/>
     </row>
     <row r="30" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A30" s="134"/>
-      <c r="B30" s="134"/>
-      <c r="C30" s="134"/>
-      <c r="D30" s="134"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="134"/>
-      <c r="I30" s="134"/>
-      <c r="J30" s="134"/>
+      <c r="A30" s="155"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
+      <c r="H30" s="155"/>
+      <c r="I30" s="155"/>
+      <c r="J30" s="155"/>
       <c r="K30" s="123"/>
       <c r="L30" s="123"/>
       <c r="M30" s="123"/>
@@ -4742,16 +4772,16 @@
       <c r="R30" s="123"/>
     </row>
     <row r="31" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A31" s="134"/>
-      <c r="B31" s="134"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="134"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="134"/>
-      <c r="I31" s="134"/>
-      <c r="J31" s="134"/>
+      <c r="A31" s="155"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="155"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="155"/>
+      <c r="G31" s="155"/>
+      <c r="H31" s="155"/>
+      <c r="I31" s="155"/>
+      <c r="J31" s="155"/>
       <c r="K31" s="123"/>
       <c r="L31" s="123"/>
       <c r="M31" s="123"/>
@@ -4763,6 +4793,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="DF28:DV28"/>
+    <mergeCell ref="DW28:EM28"/>
+    <mergeCell ref="EN28:FD28"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="FE28:FU28"/>
+    <mergeCell ref="FV28:GL28"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="Y28:AO28"/>
+    <mergeCell ref="AP28:BF28"/>
+    <mergeCell ref="BG28:BW28"/>
+    <mergeCell ref="BX28:CN28"/>
+    <mergeCell ref="CO28:DE28"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B20:R20"/>
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B19:R19"/>
     <mergeCell ref="B14:R14"/>
     <mergeCell ref="B15:R15"/>
     <mergeCell ref="A16:J16"/>
@@ -4776,28 +4828,6 @@
     <mergeCell ref="C1:F3"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B19:R19"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="FE28:FU28"/>
-    <mergeCell ref="FV28:GL28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="S28:X28"/>
-    <mergeCell ref="Y28:AO28"/>
-    <mergeCell ref="AP28:BF28"/>
-    <mergeCell ref="BG28:BW28"/>
-    <mergeCell ref="BX28:CN28"/>
-    <mergeCell ref="CO28:DE28"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="DF28:DV28"/>
-    <mergeCell ref="DW28:EM28"/>
-    <mergeCell ref="EN28:FD28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0" header="0" footer="0"/>
@@ -5336,7 +5366,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:J7"/>
+      <selection activeCell="E29" sqref="E29:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -5352,10 +5382,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
+      <c r="B1" s="162"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -5382,8 +5412,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5410,7 +5440,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="12" customHeight="1">
-      <c r="J3" s="130"/>
+      <c r="J3" s="129"/>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">
       <c r="A4" s="39" t="s">
@@ -5425,14 +5455,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="164" t="s">
+      <c r="E4" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="164"/>
-      <c r="G4" s="164"/>
-      <c r="H4" s="164"/>
-      <c r="I4" s="164"/>
-      <c r="J4" s="164"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
     </row>
     <row r="5" spans="1:10" ht="24.75" customHeight="1">
       <c r="A5" s="40">
@@ -5447,14 +5477,14 @@
       <c r="D5" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="165" t="s">
+      <c r="E5" s="164" t="s">
         <v>164</v>
       </c>
-      <c r="F5" s="156"/>
-      <c r="G5" s="156"/>
-      <c r="H5" s="156"/>
-      <c r="I5" s="156"/>
-      <c r="J5" s="156"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="165"/>
     </row>
     <row r="6" spans="1:10" ht="12.75">
       <c r="A6" s="92">
@@ -5481,12 +5511,12 @@
       </c>
       <c r="C7" s="80"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="159"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="157"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="158"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="94">
@@ -5497,12 +5527,12 @@
       </c>
       <c r="C8" s="80"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="160"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="161"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="161"/>
-      <c r="J8" s="162"/>
+      <c r="E8" s="159"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="161"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="95">
@@ -5513,12 +5543,12 @@
       </c>
       <c r="C9" s="80"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="158"/>
-      <c r="G9" s="158"/>
-      <c r="H9" s="158"/>
-      <c r="I9" s="158"/>
-      <c r="J9" s="159"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="157"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="96">
@@ -5529,12 +5559,12 @@
       </c>
       <c r="C10" s="80"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="158"/>
-      <c r="G10" s="158"/>
-      <c r="H10" s="158"/>
-      <c r="I10" s="158"/>
-      <c r="J10" s="159"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="157"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="158"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="97">
@@ -5545,12 +5575,12 @@
       </c>
       <c r="C11" s="80"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="158"/>
-      <c r="G11" s="158"/>
-      <c r="H11" s="158"/>
-      <c r="I11" s="158"/>
-      <c r="J11" s="159"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="158"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="98">
@@ -5561,12 +5591,12 @@
       </c>
       <c r="C12" s="80"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="157"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="158"/>
-      <c r="H12" s="158"/>
-      <c r="I12" s="158"/>
-      <c r="J12" s="159"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="157"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="157"/>
+      <c r="I12" s="157"/>
+      <c r="J12" s="158"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="99">
@@ -5577,12 +5607,12 @@
       </c>
       <c r="C13" s="80"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="157"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="159"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="158"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="100">
@@ -5593,12 +5623,12 @@
       </c>
       <c r="C14" s="80"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="157"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="159"/>
+      <c r="E14" s="156"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="158"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="40">
@@ -5609,12 +5639,12 @@
       </c>
       <c r="C15" s="80"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="156"/>
-      <c r="F15" s="156"/>
-      <c r="G15" s="156"/>
-      <c r="H15" s="156"/>
-      <c r="I15" s="156"/>
-      <c r="J15" s="156"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="92">
@@ -5625,12 +5655,12 @@
       </c>
       <c r="C16" s="80"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="156"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="156"/>
-      <c r="H16" s="156"/>
-      <c r="I16" s="156"/>
-      <c r="J16" s="156"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="93">
@@ -5641,12 +5671,12 @@
       </c>
       <c r="C17" s="80"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="156"/>
-      <c r="F17" s="156"/>
-      <c r="G17" s="156"/>
-      <c r="H17" s="156"/>
-      <c r="I17" s="156"/>
-      <c r="J17" s="156"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="94">
@@ -5657,12 +5687,12 @@
       </c>
       <c r="C18" s="80"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="156"/>
-      <c r="I18" s="156"/>
-      <c r="J18" s="156"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="95">
@@ -5673,12 +5703,12 @@
       </c>
       <c r="C19" s="80"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="156"/>
-      <c r="F19" s="156"/>
-      <c r="G19" s="156"/>
-      <c r="H19" s="156"/>
-      <c r="I19" s="156"/>
-      <c r="J19" s="156"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="165"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="96">
@@ -5689,12 +5719,12 @@
       </c>
       <c r="C20" s="80"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="156"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="156"/>
+      <c r="E20" s="165"/>
+      <c r="F20" s="165"/>
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165"/>
+      <c r="J20" s="165"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="97">
@@ -5705,12 +5735,12 @@
       </c>
       <c r="C21" s="80"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="156"/>
-      <c r="G21" s="156"/>
-      <c r="H21" s="156"/>
-      <c r="I21" s="156"/>
-      <c r="J21" s="156"/>
+      <c r="E21" s="165"/>
+      <c r="F21" s="165"/>
+      <c r="G21" s="165"/>
+      <c r="H21" s="165"/>
+      <c r="I21" s="165"/>
+      <c r="J21" s="165"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="98">
@@ -5721,12 +5751,12 @@
       </c>
       <c r="C22" s="80"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="156"/>
-      <c r="F22" s="156"/>
-      <c r="G22" s="156"/>
-      <c r="H22" s="156"/>
-      <c r="I22" s="156"/>
-      <c r="J22" s="156"/>
+      <c r="E22" s="165"/>
+      <c r="F22" s="165"/>
+      <c r="G22" s="165"/>
+      <c r="H22" s="165"/>
+      <c r="I22" s="165"/>
+      <c r="J22" s="165"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="99">
@@ -5737,12 +5767,12 @@
       </c>
       <c r="C23" s="80"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="156"/>
-      <c r="F23" s="156"/>
-      <c r="G23" s="156"/>
-      <c r="H23" s="156"/>
-      <c r="I23" s="156"/>
-      <c r="J23" s="156"/>
+      <c r="E23" s="165"/>
+      <c r="F23" s="165"/>
+      <c r="G23" s="165"/>
+      <c r="H23" s="165"/>
+      <c r="I23" s="165"/>
+      <c r="J23" s="165"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="100">
@@ -5753,12 +5783,12 @@
       </c>
       <c r="C24" s="80"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="156"/>
+      <c r="E24" s="165"/>
+      <c r="F24" s="165"/>
+      <c r="G24" s="165"/>
+      <c r="H24" s="165"/>
+      <c r="I24" s="165"/>
+      <c r="J24" s="165"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="40">
@@ -5769,12 +5799,12 @@
       </c>
       <c r="C25" s="80"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156"/>
-      <c r="J25" s="156"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
+      <c r="H25" s="165"/>
+      <c r="I25" s="165"/>
+      <c r="J25" s="165"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="40">
@@ -5785,12 +5815,12 @@
       </c>
       <c r="C26" s="80"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="156"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="156"/>
-      <c r="H26" s="156"/>
-      <c r="I26" s="156"/>
-      <c r="J26" s="156"/>
+      <c r="E26" s="165"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="165"/>
+      <c r="J26" s="165"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="92">
@@ -5801,12 +5831,12 @@
       </c>
       <c r="C27" s="80"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="156"/>
-      <c r="F27" s="156"/>
-      <c r="G27" s="156"/>
-      <c r="H27" s="156"/>
-      <c r="I27" s="156"/>
-      <c r="J27" s="156"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="165"/>
+      <c r="G27" s="165"/>
+      <c r="H27" s="165"/>
+      <c r="I27" s="165"/>
+      <c r="J27" s="165"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="93">
@@ -5817,12 +5847,12 @@
       </c>
       <c r="C28" s="80"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="E28" s="165"/>
+      <c r="F28" s="165"/>
+      <c r="G28" s="165"/>
+      <c r="H28" s="165"/>
+      <c r="I28" s="165"/>
+      <c r="J28" s="165"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="94">
@@ -5833,12 +5863,12 @@
       </c>
       <c r="C29" s="80"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="156"/>
-      <c r="F29" s="156"/>
-      <c r="G29" s="156"/>
-      <c r="H29" s="156"/>
-      <c r="I29" s="156"/>
-      <c r="J29" s="156"/>
+      <c r="E29" s="165"/>
+      <c r="F29" s="165"/>
+      <c r="G29" s="165"/>
+      <c r="H29" s="165"/>
+      <c r="I29" s="165"/>
+      <c r="J29" s="165"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="95">
@@ -5849,12 +5879,12 @@
       </c>
       <c r="C30" s="80"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="156"/>
-      <c r="F30" s="156"/>
-      <c r="G30" s="156"/>
-      <c r="H30" s="156"/>
-      <c r="I30" s="156"/>
-      <c r="J30" s="156"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="165"/>
+      <c r="G30" s="165"/>
+      <c r="H30" s="165"/>
+      <c r="I30" s="165"/>
+      <c r="J30" s="165"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="96">
@@ -5865,12 +5895,12 @@
       </c>
       <c r="C31" s="80"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="156"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="156"/>
-      <c r="H31" s="156"/>
-      <c r="I31" s="156"/>
-      <c r="J31" s="156"/>
+      <c r="E31" s="165"/>
+      <c r="F31" s="165"/>
+      <c r="G31" s="165"/>
+      <c r="H31" s="165"/>
+      <c r="I31" s="165"/>
+      <c r="J31" s="165"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="97">
@@ -5881,12 +5911,12 @@
       </c>
       <c r="C32" s="80"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="156"/>
-      <c r="F32" s="156"/>
-      <c r="G32" s="156"/>
-      <c r="H32" s="156"/>
-      <c r="I32" s="156"/>
-      <c r="J32" s="156"/>
+      <c r="E32" s="165"/>
+      <c r="F32" s="165"/>
+      <c r="G32" s="165"/>
+      <c r="H32" s="165"/>
+      <c r="I32" s="165"/>
+      <c r="J32" s="165"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="98">
@@ -5897,12 +5927,12 @@
       </c>
       <c r="C33" s="80"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="156"/>
-      <c r="F33" s="156"/>
-      <c r="G33" s="156"/>
-      <c r="H33" s="156"/>
-      <c r="I33" s="156"/>
-      <c r="J33" s="156"/>
+      <c r="E33" s="165"/>
+      <c r="F33" s="165"/>
+      <c r="G33" s="165"/>
+      <c r="H33" s="165"/>
+      <c r="I33" s="165"/>
+      <c r="J33" s="165"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="99">
@@ -5913,12 +5943,12 @@
       </c>
       <c r="C34" s="80"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="156"/>
-      <c r="F34" s="156"/>
-      <c r="G34" s="156"/>
-      <c r="H34" s="156"/>
-      <c r="I34" s="156"/>
-      <c r="J34" s="156"/>
+      <c r="E34" s="165"/>
+      <c r="F34" s="165"/>
+      <c r="G34" s="165"/>
+      <c r="H34" s="165"/>
+      <c r="I34" s="165"/>
+      <c r="J34" s="165"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="100">
@@ -5929,12 +5959,12 @@
       </c>
       <c r="C35" s="80"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="156"/>
-      <c r="F35" s="156"/>
-      <c r="G35" s="156"/>
-      <c r="H35" s="156"/>
-      <c r="I35" s="156"/>
-      <c r="J35" s="156"/>
+      <c r="E35" s="165"/>
+      <c r="F35" s="165"/>
+      <c r="G35" s="165"/>
+      <c r="H35" s="165"/>
+      <c r="I35" s="165"/>
+      <c r="J35" s="165"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="40">
@@ -5945,12 +5975,12 @@
       </c>
       <c r="C36" s="80"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="156"/>
-      <c r="F36" s="156"/>
-      <c r="G36" s="156"/>
-      <c r="H36" s="156"/>
-      <c r="I36" s="156"/>
-      <c r="J36" s="156"/>
+      <c r="E36" s="165"/>
+      <c r="F36" s="165"/>
+      <c r="G36" s="165"/>
+      <c r="H36" s="165"/>
+      <c r="I36" s="165"/>
+      <c r="J36" s="165"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="92">
@@ -5961,12 +5991,12 @@
       </c>
       <c r="C37" s="80"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="156"/>
-      <c r="F37" s="156"/>
-      <c r="G37" s="156"/>
-      <c r="H37" s="156"/>
-      <c r="I37" s="156"/>
-      <c r="J37" s="156"/>
+      <c r="E37" s="165"/>
+      <c r="F37" s="165"/>
+      <c r="G37" s="165"/>
+      <c r="H37" s="165"/>
+      <c r="I37" s="165"/>
+      <c r="J37" s="165"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="93">
@@ -5977,12 +6007,12 @@
       </c>
       <c r="C38" s="80"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="156"/>
-      <c r="F38" s="156"/>
-      <c r="G38" s="156"/>
-      <c r="H38" s="156"/>
-      <c r="I38" s="156"/>
-      <c r="J38" s="156"/>
+      <c r="E38" s="165"/>
+      <c r="F38" s="165"/>
+      <c r="G38" s="165"/>
+      <c r="H38" s="165"/>
+      <c r="I38" s="165"/>
+      <c r="J38" s="165"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="94">
@@ -5993,12 +6023,12 @@
       </c>
       <c r="C39" s="80"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="156"/>
-      <c r="F39" s="156"/>
-      <c r="G39" s="156"/>
-      <c r="H39" s="156"/>
-      <c r="I39" s="156"/>
-      <c r="J39" s="156"/>
+      <c r="E39" s="165"/>
+      <c r="F39" s="165"/>
+      <c r="G39" s="165"/>
+      <c r="H39" s="165"/>
+      <c r="I39" s="165"/>
+      <c r="J39" s="165"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="95">
@@ -6009,12 +6039,12 @@
       </c>
       <c r="C40" s="80"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="156"/>
-      <c r="F40" s="156"/>
-      <c r="G40" s="156"/>
-      <c r="H40" s="156"/>
-      <c r="I40" s="156"/>
-      <c r="J40" s="156"/>
+      <c r="E40" s="165"/>
+      <c r="F40" s="165"/>
+      <c r="G40" s="165"/>
+      <c r="H40" s="165"/>
+      <c r="I40" s="165"/>
+      <c r="J40" s="165"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="96">
@@ -6025,12 +6055,12 @@
       </c>
       <c r="C41" s="80"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="156"/>
-      <c r="F41" s="156"/>
-      <c r="G41" s="156"/>
-      <c r="H41" s="156"/>
-      <c r="I41" s="156"/>
-      <c r="J41" s="156"/>
+      <c r="E41" s="165"/>
+      <c r="F41" s="165"/>
+      <c r="G41" s="165"/>
+      <c r="H41" s="165"/>
+      <c r="I41" s="165"/>
+      <c r="J41" s="165"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="97">
@@ -6041,23 +6071,32 @@
       </c>
       <c r="C42" s="80"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="156"/>
-      <c r="F42" s="156"/>
-      <c r="G42" s="156"/>
-      <c r="H42" s="156"/>
-      <c r="I42" s="156"/>
-      <c r="J42" s="156"/>
+      <c r="E42" s="165"/>
+      <c r="F42" s="165"/>
+      <c r="G42" s="165"/>
+      <c r="H42" s="165"/>
+      <c r="I42" s="165"/>
+      <c r="J42" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -6073,23 +6112,14 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -6114,7 +6144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I12" sqref="I12:J43"/>
     </sheetView>
   </sheetViews>
@@ -6134,10 +6164,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
+      <c r="B1" s="162"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -6165,8 +6195,8 @@
       <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -6307,7 +6337,7 @@
       <c r="G12" s="43"/>
       <c r="H12" s="45"/>
       <c r="I12" s="172" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J12" s="173"/>
     </row>
@@ -6738,11 +6768,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -6766,12 +6796,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
       <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6801,10 +6831,10 @@
       <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
       <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6926,7 +6956,7 @@
         <v>198</v>
       </c>
       <c r="E6" s="89" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="F6" s="128" t="s">
         <v>179</v>
@@ -6943,7 +6973,9 @@
       <c r="L6" s="70"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="89"/>
+      <c r="O6" s="89" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="7" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="190"/>
@@ -7314,7 +7346,7 @@
       <c r="B18" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="130" t="s">
         <v>168</v>
       </c>
       <c r="D18" s="59" t="s">
@@ -7346,20 +7378,38 @@
       <c r="A19" s="33">
         <v>14</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="131"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+      <c r="B19" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="33">
+        <v>4</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="E19" s="132" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>190</v>
+      </c>
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
+      <c r="K19" s="40" t="s">
+        <v>193</v>
+      </c>
       <c r="L19" s="40"/>
       <c r="M19" s="40"/>
       <c r="N19" s="70"/>
-      <c r="O19" s="89"/>
+      <c r="O19" s="89" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="20" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="33">
@@ -9067,7 +9117,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="198" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="126"/>
@@ -9100,7 +9150,7 @@
       <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="196"/>
+      <c r="A2" s="199"/>
       <c r="B2" s="127"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
@@ -9146,15 +9196,15 @@
       <c r="E4" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="163" t="s">
+      <c r="F4" s="162" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163" t="s">
+      <c r="G4" s="162"/>
+      <c r="H4" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
+      <c r="I4" s="162"/>
+      <c r="J4" s="162"/>
     </row>
     <row r="5" spans="1:12" s="34" customFormat="1" ht="25.5" customHeight="1">
       <c r="A5" s="33">
@@ -9164,19 +9214,19 @@
         <v>167</v>
       </c>
       <c r="C5" s="33"/>
-      <c r="D5" s="132" t="s">
+      <c r="D5" s="130" t="s">
         <v>135</v>
       </c>
       <c r="E5" s="32"/>
-      <c r="F5" s="193" t="s">
-        <v>209</v>
-      </c>
-      <c r="G5" s="194"/>
-      <c r="H5" s="197" t="s">
-        <v>210</v>
-      </c>
-      <c r="I5" s="198"/>
-      <c r="J5" s="199"/>
+      <c r="F5" s="196" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="197"/>
+      <c r="H5" s="193" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="194"/>
+      <c r="J5" s="195"/>
     </row>
     <row r="6" spans="1:12" s="34" customFormat="1" ht="11.25">
       <c r="A6" s="33">
@@ -9186,11 +9236,11 @@
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
       <c r="E6" s="32"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="197"/>
-      <c r="I6" s="198"/>
-      <c r="J6" s="199"/>
+      <c r="F6" s="196"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="195"/>
     </row>
     <row r="7" spans="1:12" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A7" s="33">
@@ -9200,11 +9250,11 @@
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="193"/>
-      <c r="G7" s="194"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="198"/>
-      <c r="J7" s="199"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="194"/>
+      <c r="J7" s="195"/>
     </row>
     <row r="8" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="33">
@@ -9214,11 +9264,11 @@
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="193"/>
-      <c r="G8" s="194"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="198"/>
-      <c r="J8" s="199"/>
+      <c r="F8" s="196"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="193"/>
+      <c r="I8" s="194"/>
+      <c r="J8" s="195"/>
     </row>
     <row r="9" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="33">
@@ -9228,11 +9278,11 @@
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="198"/>
-      <c r="J9" s="199"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="194"/>
+      <c r="J9" s="195"/>
     </row>
     <row r="10" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="33">
@@ -9242,11 +9292,11 @@
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="198"/>
-      <c r="J10" s="199"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="193"/>
+      <c r="I10" s="194"/>
+      <c r="J10" s="195"/>
     </row>
     <row r="11" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="33">
@@ -9256,11 +9306,11 @@
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="194"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="198"/>
-      <c r="J11" s="199"/>
+      <c r="F11" s="196"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="193"/>
+      <c r="I11" s="194"/>
+      <c r="J11" s="195"/>
     </row>
     <row r="12" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="33">
@@ -9270,11 +9320,11 @@
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="197"/>
-      <c r="I12" s="198"/>
-      <c r="J12" s="199"/>
+      <c r="F12" s="196"/>
+      <c r="G12" s="197"/>
+      <c r="H12" s="193"/>
+      <c r="I12" s="194"/>
+      <c r="J12" s="195"/>
     </row>
     <row r="13" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -9284,11 +9334,11 @@
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="193"/>
-      <c r="G13" s="194"/>
-      <c r="H13" s="197"/>
-      <c r="I13" s="198"/>
-      <c r="J13" s="199"/>
+      <c r="F13" s="196"/>
+      <c r="G13" s="197"/>
+      <c r="H13" s="193"/>
+      <c r="I13" s="194"/>
+      <c r="J13" s="195"/>
     </row>
     <row r="14" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -9298,11 +9348,11 @@
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="193"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="197"/>
-      <c r="I14" s="198"/>
-      <c r="J14" s="199"/>
+      <c r="F14" s="196"/>
+      <c r="G14" s="197"/>
+      <c r="H14" s="193"/>
+      <c r="I14" s="194"/>
+      <c r="J14" s="195"/>
     </row>
     <row r="15" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -9312,11 +9362,11 @@
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="193"/>
-      <c r="G15" s="194"/>
-      <c r="H15" s="197"/>
-      <c r="I15" s="198"/>
-      <c r="J15" s="199"/>
+      <c r="F15" s="196"/>
+      <c r="G15" s="197"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="194"/>
+      <c r="J15" s="195"/>
     </row>
     <row r="16" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="33">
@@ -9326,11 +9376,11 @@
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="32"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="194"/>
-      <c r="H16" s="197"/>
-      <c r="I16" s="198"/>
-      <c r="J16" s="199"/>
+      <c r="F16" s="196"/>
+      <c r="G16" s="197"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="194"/>
+      <c r="J16" s="195"/>
     </row>
     <row r="17" spans="1:18" s="34" customFormat="1" ht="11.25">
       <c r="A17" s="33">
@@ -9340,11 +9390,11 @@
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="32"/>
-      <c r="F17" s="193"/>
-      <c r="G17" s="194"/>
-      <c r="H17" s="197"/>
-      <c r="I17" s="198"/>
-      <c r="J17" s="199"/>
+      <c r="F17" s="196"/>
+      <c r="G17" s="197"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="194"/>
+      <c r="J17" s="195"/>
     </row>
     <row r="18" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -9354,11 +9404,11 @@
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="32"/>
-      <c r="F18" s="193"/>
-      <c r="G18" s="194"/>
-      <c r="H18" s="197"/>
-      <c r="I18" s="198"/>
-      <c r="J18" s="199"/>
+      <c r="F18" s="196"/>
+      <c r="G18" s="197"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="194"/>
+      <c r="J18" s="195"/>
     </row>
     <row r="19" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -9368,11 +9418,11 @@
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="32"/>
-      <c r="F19" s="193"/>
-      <c r="G19" s="194"/>
-      <c r="H19" s="197"/>
-      <c r="I19" s="198"/>
-      <c r="J19" s="199"/>
+      <c r="F19" s="196"/>
+      <c r="G19" s="197"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="194"/>
+      <c r="J19" s="195"/>
     </row>
     <row r="20" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="33">
@@ -9382,11 +9432,11 @@
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="193"/>
-      <c r="G20" s="194"/>
-      <c r="H20" s="197"/>
-      <c r="I20" s="198"/>
-      <c r="J20" s="199"/>
+      <c r="F20" s="196"/>
+      <c r="G20" s="197"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="194"/>
+      <c r="J20" s="195"/>
     </row>
     <row r="21" spans="1:18" s="34" customFormat="1" ht="11.25">
       <c r="A21" s="33">
@@ -9396,11 +9446,11 @@
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="193"/>
-      <c r="G21" s="194"/>
-      <c r="H21" s="197"/>
-      <c r="I21" s="198"/>
-      <c r="J21" s="199"/>
+      <c r="F21" s="196"/>
+      <c r="G21" s="197"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="194"/>
+      <c r="J21" s="195"/>
     </row>
     <row r="22" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
@@ -9410,11 +9460,11 @@
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="32"/>
-      <c r="F22" s="157"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="197"/>
-      <c r="I22" s="198"/>
-      <c r="J22" s="199"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="193"/>
+      <c r="I22" s="194"/>
+      <c r="J22" s="195"/>
     </row>
     <row r="23" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
@@ -9424,11 +9474,11 @@
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="159"/>
-      <c r="H23" s="197"/>
-      <c r="I23" s="198"/>
-      <c r="J23" s="199"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="158"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="194"/>
+      <c r="J23" s="195"/>
     </row>
     <row r="24" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
@@ -9438,11 +9488,11 @@
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="32"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="197"/>
-      <c r="I24" s="198"/>
-      <c r="J24" s="199"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="158"/>
+      <c r="H24" s="193"/>
+      <c r="I24" s="194"/>
+      <c r="J24" s="195"/>
     </row>
     <row r="25" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
@@ -9452,11 +9502,11 @@
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="159"/>
-      <c r="H25" s="197"/>
-      <c r="I25" s="198"/>
-      <c r="J25" s="199"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="194"/>
+      <c r="J25" s="195"/>
     </row>
     <row r="26" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
@@ -9466,11 +9516,11 @@
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="157"/>
-      <c r="G26" s="159"/>
-      <c r="H26" s="197"/>
-      <c r="I26" s="198"/>
-      <c r="J26" s="199"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="193"/>
+      <c r="I26" s="194"/>
+      <c r="J26" s="195"/>
     </row>
     <row r="27" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
@@ -9480,11 +9530,11 @@
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="159"/>
-      <c r="H27" s="197"/>
-      <c r="I27" s="198"/>
-      <c r="J27" s="199"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="158"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="194"/>
+      <c r="J27" s="195"/>
     </row>
     <row r="28" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
@@ -9494,11 +9544,11 @@
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="197"/>
-      <c r="I28" s="198"/>
-      <c r="J28" s="199"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="194"/>
+      <c r="J28" s="195"/>
     </row>
     <row r="29" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33">
@@ -9508,11 +9558,11 @@
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
-      <c r="F29" s="157"/>
-      <c r="G29" s="159"/>
-      <c r="H29" s="197"/>
-      <c r="I29" s="198"/>
-      <c r="J29" s="199"/>
+      <c r="F29" s="156"/>
+      <c r="G29" s="158"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="194"/>
+      <c r="J29" s="195"/>
     </row>
     <row r="30" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A30" s="33">
@@ -9522,11 +9572,11 @@
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="157"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="197"/>
-      <c r="I30" s="198"/>
-      <c r="J30" s="199"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="158"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="194"/>
+      <c r="J30" s="195"/>
     </row>
     <row r="31" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A31" s="33">
@@ -9536,11 +9586,11 @@
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="197"/>
-      <c r="I31" s="198"/>
-      <c r="J31" s="199"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="158"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="194"/>
+      <c r="J31" s="195"/>
     </row>
     <row r="32" spans="1:18" ht="11.25">
       <c r="A32" s="33">
@@ -9550,11 +9600,11 @@
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="197"/>
-      <c r="I32" s="198"/>
-      <c r="J32" s="199"/>
+      <c r="F32" s="156"/>
+      <c r="G32" s="158"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="194"/>
+      <c r="J32" s="195"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
@@ -9571,11 +9621,11 @@
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="159"/>
-      <c r="H33" s="197"/>
-      <c r="I33" s="198"/>
-      <c r="J33" s="199"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="158"/>
+      <c r="H33" s="193"/>
+      <c r="I33" s="194"/>
+      <c r="J33" s="195"/>
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
@@ -9592,11 +9642,11 @@
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
-      <c r="F34" s="157"/>
-      <c r="G34" s="159"/>
-      <c r="H34" s="197"/>
-      <c r="I34" s="198"/>
-      <c r="J34" s="199"/>
+      <c r="F34" s="156"/>
+      <c r="G34" s="158"/>
+      <c r="H34" s="193"/>
+      <c r="I34" s="194"/>
+      <c r="J34" s="195"/>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
@@ -9613,11 +9663,11 @@
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
-      <c r="F35" s="157"/>
-      <c r="G35" s="159"/>
-      <c r="H35" s="197"/>
-      <c r="I35" s="198"/>
-      <c r="J35" s="199"/>
+      <c r="F35" s="156"/>
+      <c r="G35" s="158"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="194"/>
+      <c r="J35" s="195"/>
       <c r="L35" s="22"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
@@ -9634,11 +9684,11 @@
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="32"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="159"/>
-      <c r="H36" s="197"/>
-      <c r="I36" s="198"/>
-      <c r="J36" s="199"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="158"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="194"/>
+      <c r="J36" s="195"/>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
@@ -9655,11 +9705,11 @@
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
-      <c r="F37" s="157"/>
-      <c r="G37" s="159"/>
-      <c r="H37" s="197"/>
-      <c r="I37" s="198"/>
-      <c r="J37" s="199"/>
+      <c r="F37" s="156"/>
+      <c r="G37" s="158"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="194"/>
+      <c r="J37" s="195"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
@@ -9676,11 +9726,11 @@
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="32"/>
-      <c r="F38" s="157"/>
-      <c r="G38" s="159"/>
-      <c r="H38" s="197"/>
-      <c r="I38" s="198"/>
-      <c r="J38" s="199"/>
+      <c r="F38" s="156"/>
+      <c r="G38" s="158"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="194"/>
+      <c r="J38" s="195"/>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
@@ -9697,11 +9747,11 @@
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="157"/>
-      <c r="G39" s="159"/>
-      <c r="H39" s="197"/>
-      <c r="I39" s="198"/>
-      <c r="J39" s="199"/>
+      <c r="F39" s="156"/>
+      <c r="G39" s="158"/>
+      <c r="H39" s="193"/>
+      <c r="I39" s="194"/>
+      <c r="J39" s="195"/>
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
@@ -9718,11 +9768,11 @@
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="32"/>
-      <c r="F40" s="157"/>
-      <c r="G40" s="159"/>
-      <c r="H40" s="197"/>
-      <c r="I40" s="198"/>
-      <c r="J40" s="199"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="158"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="194"/>
+      <c r="J40" s="195"/>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
@@ -9739,11 +9789,11 @@
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
-      <c r="F41" s="157"/>
-      <c r="G41" s="159"/>
-      <c r="H41" s="197"/>
-      <c r="I41" s="198"/>
-      <c r="J41" s="199"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="158"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="194"/>
+      <c r="J41" s="195"/>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
@@ -9760,11 +9810,11 @@
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="32"/>
-      <c r="F42" s="157"/>
-      <c r="G42" s="159"/>
-      <c r="H42" s="197"/>
-      <c r="I42" s="198"/>
-      <c r="J42" s="199"/>
+      <c r="F42" s="156"/>
+      <c r="G42" s="158"/>
+      <c r="H42" s="193"/>
+      <c r="I42" s="194"/>
+      <c r="J42" s="195"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
@@ -9781,11 +9831,11 @@
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="32"/>
-      <c r="F43" s="157"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="197"/>
-      <c r="I43" s="198"/>
-      <c r="J43" s="199"/>
+      <c r="F43" s="156"/>
+      <c r="G43" s="158"/>
+      <c r="H43" s="193"/>
+      <c r="I43" s="194"/>
+      <c r="J43" s="195"/>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
@@ -9802,11 +9852,11 @@
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
       <c r="E44" s="32"/>
-      <c r="F44" s="157"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="197"/>
-      <c r="I44" s="198"/>
-      <c r="J44" s="199"/>
+      <c r="F44" s="156"/>
+      <c r="G44" s="158"/>
+      <c r="H44" s="193"/>
+      <c r="I44" s="194"/>
+      <c r="J44" s="195"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
@@ -9823,11 +9873,11 @@
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
       <c r="E45" s="32"/>
-      <c r="F45" s="157"/>
-      <c r="G45" s="159"/>
-      <c r="H45" s="197"/>
-      <c r="I45" s="198"/>
-      <c r="J45" s="199"/>
+      <c r="F45" s="156"/>
+      <c r="G45" s="158"/>
+      <c r="H45" s="193"/>
+      <c r="I45" s="194"/>
+      <c r="J45" s="195"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
@@ -9844,11 +9894,11 @@
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
       <c r="E46" s="32"/>
-      <c r="F46" s="157"/>
-      <c r="G46" s="159"/>
-      <c r="H46" s="197"/>
-      <c r="I46" s="198"/>
-      <c r="J46" s="199"/>
+      <c r="F46" s="156"/>
+      <c r="G46" s="158"/>
+      <c r="H46" s="193"/>
+      <c r="I46" s="194"/>
+      <c r="J46" s="195"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
@@ -9865,11 +9915,11 @@
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="32"/>
-      <c r="F47" s="157"/>
-      <c r="G47" s="159"/>
-      <c r="H47" s="197"/>
-      <c r="I47" s="198"/>
-      <c r="J47" s="199"/>
+      <c r="F47" s="156"/>
+      <c r="G47" s="158"/>
+      <c r="H47" s="193"/>
+      <c r="I47" s="194"/>
+      <c r="J47" s="195"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
@@ -9886,11 +9936,11 @@
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="32"/>
-      <c r="F48" s="157"/>
-      <c r="G48" s="159"/>
-      <c r="H48" s="197"/>
-      <c r="I48" s="198"/>
-      <c r="J48" s="199"/>
+      <c r="F48" s="156"/>
+      <c r="G48" s="158"/>
+      <c r="H48" s="193"/>
+      <c r="I48" s="194"/>
+      <c r="J48" s="195"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
@@ -9907,11 +9957,11 @@
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
-      <c r="F49" s="157"/>
-      <c r="G49" s="159"/>
-      <c r="H49" s="197"/>
-      <c r="I49" s="198"/>
-      <c r="J49" s="199"/>
+      <c r="F49" s="156"/>
+      <c r="G49" s="158"/>
+      <c r="H49" s="193"/>
+      <c r="I49" s="194"/>
+      <c r="J49" s="195"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
@@ -9928,11 +9978,11 @@
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="32"/>
-      <c r="F50" s="157"/>
-      <c r="G50" s="159"/>
-      <c r="H50" s="197"/>
-      <c r="I50" s="198"/>
-      <c r="J50" s="199"/>
+      <c r="F50" s="156"/>
+      <c r="G50" s="158"/>
+      <c r="H50" s="193"/>
+      <c r="I50" s="194"/>
+      <c r="J50" s="195"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
@@ -9949,11 +9999,11 @@
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="32"/>
-      <c r="F51" s="157"/>
-      <c r="G51" s="159"/>
-      <c r="H51" s="197"/>
-      <c r="I51" s="198"/>
-      <c r="J51" s="199"/>
+      <c r="F51" s="156"/>
+      <c r="G51" s="158"/>
+      <c r="H51" s="193"/>
+      <c r="I51" s="194"/>
+      <c r="J51" s="195"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
@@ -9970,11 +10020,11 @@
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="32"/>
-      <c r="F52" s="157"/>
-      <c r="G52" s="159"/>
-      <c r="H52" s="197"/>
-      <c r="I52" s="198"/>
-      <c r="J52" s="199"/>
+      <c r="F52" s="156"/>
+      <c r="G52" s="158"/>
+      <c r="H52" s="193"/>
+      <c r="I52" s="194"/>
+      <c r="J52" s="195"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
@@ -9991,11 +10041,11 @@
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="157"/>
-      <c r="G53" s="159"/>
-      <c r="H53" s="197"/>
-      <c r="I53" s="198"/>
-      <c r="J53" s="199"/>
+      <c r="F53" s="156"/>
+      <c r="G53" s="158"/>
+      <c r="H53" s="193"/>
+      <c r="I53" s="194"/>
+      <c r="J53" s="195"/>
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
@@ -10012,11 +10062,11 @@
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="32"/>
-      <c r="F54" s="157"/>
-      <c r="G54" s="159"/>
-      <c r="H54" s="197"/>
-      <c r="I54" s="198"/>
-      <c r="J54" s="199"/>
+      <c r="F54" s="156"/>
+      <c r="G54" s="158"/>
+      <c r="H54" s="193"/>
+      <c r="I54" s="194"/>
+      <c r="J54" s="195"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
@@ -10033,11 +10083,11 @@
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="32"/>
-      <c r="F55" s="157"/>
-      <c r="G55" s="159"/>
-      <c r="H55" s="197"/>
-      <c r="I55" s="198"/>
-      <c r="J55" s="199"/>
+      <c r="F55" s="156"/>
+      <c r="G55" s="158"/>
+      <c r="H55" s="193"/>
+      <c r="I55" s="194"/>
+      <c r="J55" s="195"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
@@ -10054,11 +10104,11 @@
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
       <c r="E56" s="32"/>
-      <c r="F56" s="157"/>
-      <c r="G56" s="159"/>
-      <c r="H56" s="197"/>
-      <c r="I56" s="198"/>
-      <c r="J56" s="199"/>
+      <c r="F56" s="156"/>
+      <c r="G56" s="158"/>
+      <c r="H56" s="193"/>
+      <c r="I56" s="194"/>
+      <c r="J56" s="195"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
@@ -10070,6 +10120,99 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="107">
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="H49:J49"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="F54:G54"/>
@@ -10084,99 +10227,6 @@
     <mergeCell ref="H54:J54"/>
     <mergeCell ref="H55:J55"/>
     <mergeCell ref="H56:J56"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E56">
@@ -10195,7 +10245,7 @@
   <dimension ref="A1:T1048467"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="G4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:R5"/>
+      <selection activeCell="J5" sqref="J5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -10214,7 +10264,8 @@
     <col min="12" max="12" width="15.28515625" style="23" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" style="23" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" style="23" customWidth="1"/>
-    <col min="15" max="17" width="14.140625" style="23" customWidth="1"/>
+    <col min="15" max="15" width="17" style="23" customWidth="1"/>
+    <col min="16" max="17" width="14.140625" style="23" customWidth="1"/>
     <col min="18" max="18" width="36.7109375" style="23" customWidth="1"/>
     <col min="19" max="20" width="12.7109375" style="23" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" style="22" customWidth="1"/>
@@ -10222,23 +10273,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
       <c r="H1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="206" t="str">
+      <c r="I1" s="203" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="J1" s="206"/>
+      <c r="J1" s="203"/>
       <c r="K1" s="26" t="s">
         <v>3</v>
       </c>
@@ -10263,21 +10314,21 @@
       <c r="T1" s="52"/>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
       <c r="H2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="206" t="str">
+      <c r="I2" s="203" t="str">
         <f>'Update History'!D2</f>
         <v>ASSOFT - CRM</v>
       </c>
-      <c r="J2" s="206"/>
+      <c r="J2" s="203"/>
       <c r="K2" s="26" t="s">
         <v>49</v>
       </c>
@@ -10351,7 +10402,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="34" customFormat="1" ht="132.75" customHeight="1">
+    <row r="5" spans="1:20" s="34" customFormat="1" ht="181.5" customHeight="1">
       <c r="A5" s="33">
         <v>1</v>
       </c>
@@ -10370,29 +10421,29 @@
       <c r="H5" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="133" t="s">
+      <c r="I5" s="131" t="s">
         <v>202</v>
       </c>
       <c r="J5" s="200" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="K5" s="201"/>
       <c r="L5" s="201"/>
       <c r="M5" s="202"/>
-      <c r="N5" s="129" t="s">
-        <v>204</v>
-      </c>
-      <c r="O5" s="129" t="s">
-        <v>205</v>
+      <c r="N5" s="133" t="s">
+        <v>211</v>
+      </c>
+      <c r="O5" s="133" t="s">
+        <v>212</v>
       </c>
       <c r="P5" s="77" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="Q5" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="R5" s="89" t="s">
-        <v>208</v>
+        <v>203</v>
+      </c>
+      <c r="R5" s="132" t="s">
+        <v>214</v>
       </c>
       <c r="S5" s="64"/>
       <c r="T5" s="64"/>
@@ -10441,7 +10492,7 @@
       <c r="O7" s="90"/>
       <c r="P7" s="77"/>
       <c r="Q7" s="76"/>
-      <c r="R7" s="203"/>
+      <c r="R7" s="204"/>
       <c r="S7" s="64"/>
       <c r="T7" s="64"/>
     </row>
@@ -10465,7 +10516,7 @@
       <c r="O8" s="90"/>
       <c r="P8" s="77"/>
       <c r="Q8" s="76"/>
-      <c r="R8" s="204"/>
+      <c r="R8" s="205"/>
       <c r="S8" s="64"/>
       <c r="T8" s="64"/>
     </row>
@@ -10489,7 +10540,7 @@
       <c r="O9" s="90"/>
       <c r="P9" s="77"/>
       <c r="Q9" s="76"/>
-      <c r="R9" s="205"/>
+      <c r="R9" s="206"/>
       <c r="S9" s="64"/>
       <c r="T9" s="64"/>
     </row>
@@ -10513,7 +10564,7 @@
       <c r="O10" s="90"/>
       <c r="P10" s="77"/>
       <c r="Q10" s="76"/>
-      <c r="R10" s="203"/>
+      <c r="R10" s="204"/>
       <c r="S10" s="64"/>
       <c r="T10" s="64"/>
     </row>
@@ -10537,7 +10588,7 @@
       <c r="O11" s="90"/>
       <c r="P11" s="77"/>
       <c r="Q11" s="76"/>
-      <c r="R11" s="204"/>
+      <c r="R11" s="205"/>
       <c r="S11" s="64"/>
       <c r="T11" s="64"/>
     </row>
@@ -10561,7 +10612,7 @@
       <c r="O12" s="86"/>
       <c r="P12" s="77"/>
       <c r="Q12" s="76"/>
-      <c r="R12" s="204"/>
+      <c r="R12" s="205"/>
       <c r="S12" s="64"/>
       <c r="T12" s="64"/>
     </row>
@@ -10585,7 +10636,7 @@
       <c r="O13" s="86"/>
       <c r="P13" s="77"/>
       <c r="Q13" s="76"/>
-      <c r="R13" s="205"/>
+      <c r="R13" s="206"/>
       <c r="S13" s="64"/>
       <c r="T13" s="64"/>
     </row>
@@ -12477,60 +12528,32 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="96">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J88:M88"/>
+    <mergeCell ref="J89:M89"/>
+    <mergeCell ref="J90:M90"/>
+    <mergeCell ref="J91:M91"/>
+    <mergeCell ref="J92:M92"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R10:R13"/>
+    <mergeCell ref="J87:M87"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J67:M67"/>
+    <mergeCell ref="J68:M68"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J72:M72"/>
+    <mergeCell ref="J73:M73"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="J76:M76"/>
     <mergeCell ref="J93:M93"/>
     <mergeCell ref="J94:M94"/>
     <mergeCell ref="J5:M5"/>
@@ -12547,32 +12570,60 @@
     <mergeCell ref="J69:M69"/>
     <mergeCell ref="J70:M70"/>
     <mergeCell ref="J71:M71"/>
-    <mergeCell ref="J72:M72"/>
-    <mergeCell ref="J73:M73"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="J77:M77"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R10:R13"/>
-    <mergeCell ref="J87:M87"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J67:M67"/>
-    <mergeCell ref="J68:M68"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J88:M88"/>
-    <mergeCell ref="J89:M89"/>
-    <mergeCell ref="J90:M90"/>
-    <mergeCell ref="J91:M91"/>
-    <mergeCell ref="J92:M92"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J11:M11"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="P1048467:P1048576 P5:P94"/>
@@ -12601,8 +12652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A37" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -12618,10 +12669,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
+      <c r="B1" s="162"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -12649,8 +12700,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13220,7 +13271,7 @@
     </row>
     <row r="49" spans="1:10" ht="12" customHeight="1">
       <c r="B49" s="81" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C49" s="87"/>
       <c r="D49" s="43"/>
@@ -13718,10 +13769,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
+      <c r="B1" s="162"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13749,8 +13800,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>